<commit_message>
Favicon en logo klaar
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29380B0-D458-4033-9778-1D0AFA85F4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE33BD08-66E5-4960-8DB1-E9C083377BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="870" windowWidth="14400" windowHeight="7810" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,9 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -993,199 +990,199 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>51</c:v>
+                  <c:v>48.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2870,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2884,172 +2881,172 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:79" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="21"/>
-      <c r="AT2" s="21"/>
-      <c r="AU2" s="21"/>
-      <c r="AV2" s="21"/>
-      <c r="AW2" s="21"/>
-      <c r="AX2" s="21"/>
-      <c r="AY2" s="21"/>
-      <c r="AZ2" s="21"/>
-      <c r="BA2" s="21"/>
-      <c r="BB2" s="21"/>
-      <c r="BC2" s="21"/>
-      <c r="BD2" s="21"/>
-      <c r="BE2" s="21"/>
-      <c r="BF2" s="21"/>
-      <c r="BG2" s="21"/>
-      <c r="BH2" s="21"/>
-      <c r="BI2" s="21"/>
-      <c r="BJ2" s="21"/>
-      <c r="BK2" s="21"/>
-      <c r="BL2" s="21"/>
-      <c r="BM2" s="21"/>
-      <c r="BN2" s="21"/>
-      <c r="BO2" s="21"/>
-      <c r="BP2" s="21"/>
-      <c r="BQ2" s="21"/>
-      <c r="BR2" s="21"/>
-      <c r="BS2" s="21"/>
-      <c r="BT2" s="21"/>
-      <c r="BU2" s="21"/>
-      <c r="BV2" s="21"/>
-      <c r="BW2" s="21"/>
-      <c r="BX2" s="21"/>
-      <c r="BY2" s="21"/>
-      <c r="BZ2" s="21"/>
-      <c r="CA2" s="21"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="20"/>
+      <c r="BD2" s="20"/>
+      <c r="BE2" s="20"/>
+      <c r="BF2" s="20"/>
+      <c r="BG2" s="20"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
+      <c r="BK2" s="20"/>
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="20"/>
+      <c r="BN2" s="20"/>
+      <c r="BO2" s="20"/>
+      <c r="BP2" s="20"/>
+      <c r="BQ2" s="20"/>
+      <c r="BR2" s="20"/>
+      <c r="BS2" s="20"/>
+      <c r="BT2" s="20"/>
+      <c r="BU2" s="20"/>
+      <c r="BV2" s="20"/>
+      <c r="BW2" s="20"/>
+      <c r="BX2" s="20"/>
+      <c r="BY2" s="20"/>
+      <c r="BZ2" s="20"/>
+      <c r="CA2" s="20"/>
     </row>
     <row r="3" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="21"/>
-      <c r="AD3" s="21"/>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21"/>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="21"/>
-      <c r="AP3" s="21"/>
-      <c r="AQ3" s="21"/>
-      <c r="AR3" s="21"/>
-      <c r="AS3" s="21"/>
-      <c r="AT3" s="21"/>
-      <c r="AU3" s="21"/>
-      <c r="AV3" s="21"/>
-      <c r="AW3" s="21"/>
-      <c r="AX3" s="21"/>
-      <c r="AY3" s="21"/>
-      <c r="AZ3" s="21"/>
-      <c r="BA3" s="21"/>
-      <c r="BB3" s="21"/>
-      <c r="BC3" s="21"/>
-      <c r="BD3" s="21"/>
-      <c r="BE3" s="21"/>
-      <c r="BF3" s="21"/>
-      <c r="BG3" s="21"/>
-      <c r="BH3" s="21"/>
-      <c r="BI3" s="21"/>
-      <c r="BJ3" s="21"/>
-      <c r="BK3" s="21"/>
-      <c r="BL3" s="21"/>
-      <c r="BM3" s="21"/>
-      <c r="BN3" s="21"/>
-      <c r="BO3" s="21"/>
-      <c r="BP3" s="21"/>
-      <c r="BQ3" s="21"/>
-      <c r="BR3" s="21"/>
-      <c r="BS3" s="21"/>
-      <c r="BT3" s="21"/>
-      <c r="BU3" s="21"/>
-      <c r="BV3" s="21"/>
-      <c r="BW3" s="21"/>
-      <c r="BX3" s="21"/>
-      <c r="BY3" s="21"/>
-      <c r="BZ3" s="21"/>
-      <c r="CA3" s="21"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="20"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+      <c r="BB3" s="20"/>
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="20"/>
+      <c r="BE3" s="20"/>
+      <c r="BF3" s="20"/>
+      <c r="BG3" s="20"/>
+      <c r="BH3" s="20"/>
+      <c r="BI3" s="20"/>
+      <c r="BJ3" s="20"/>
+      <c r="BK3" s="20"/>
+      <c r="BL3" s="20"/>
+      <c r="BM3" s="20"/>
+      <c r="BN3" s="20"/>
+      <c r="BO3" s="20"/>
+      <c r="BP3" s="20"/>
+      <c r="BQ3" s="20"/>
+      <c r="BR3" s="20"/>
+      <c r="BS3" s="20"/>
+      <c r="BT3" s="20"/>
+      <c r="BU3" s="20"/>
+      <c r="BV3" s="20"/>
+      <c r="BW3" s="20"/>
+      <c r="BX3" s="20"/>
+      <c r="BY3" s="20"/>
+      <c r="BZ3" s="20"/>
+      <c r="CA3" s="20"/>
     </row>
     <row r="4" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -3282,8 +3279,8 @@
       </c>
     </row>
     <row r="5" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
@@ -3517,10 +3514,10 @@
       <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>2</v>
       </c>
       <c r="E6" s="1"/>
@@ -3607,23 +3604,25 @@
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="18">
         <v>2</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19">
+        <v>0.5</v>
+      </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
@@ -3781,10 +3780,10 @@
       <c r="B9" s="5">
         <v>4</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>1</v>
       </c>
       <c r="E9" s="1"/>
@@ -3869,10 +3868,10 @@
       <c r="B10" s="5">
         <v>5</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>0.5</v>
       </c>
       <c r="E10" s="1"/>
@@ -3957,10 +3956,10 @@
       <c r="B11" s="5">
         <v>6</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>0.5</v>
       </c>
       <c r="E11" s="1"/>
@@ -4045,25 +4044,25 @@
       <c r="B12" s="5">
         <v>7</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>4</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20">
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19">
         <v>1</v>
       </c>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
@@ -4133,10 +4132,10 @@
       <c r="B13" s="5">
         <v>8</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>1</v>
       </c>
       <c r="E13" s="1"/>
@@ -4221,23 +4220,25 @@
       <c r="B14" s="5">
         <v>9</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="13">
         <v>1</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1">
+        <v>1</v>
+      </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
@@ -4307,10 +4308,10 @@
       <c r="B15" s="5">
         <v>10</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>2</v>
       </c>
       <c r="E15" s="1"/>
@@ -4395,23 +4396,23 @@
       <c r="B16" s="5">
         <v>11</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="18">
         <v>2</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
@@ -4481,7 +4482,7 @@
       <c r="B17" s="5">
         <v>12</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>88</v>
       </c>
       <c r="D17" s="12">
@@ -4567,7 +4568,7 @@
       <c r="B18" s="5">
         <v>13</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>89</v>
       </c>
       <c r="D18" s="12">
@@ -4653,23 +4654,23 @@
       <c r="B19" s="5">
         <v>14</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="18">
         <v>2</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
@@ -4739,10 +4740,10 @@
       <c r="B20" s="5">
         <v>15</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="13">
         <v>1</v>
       </c>
       <c r="E20" s="1"/>
@@ -4827,23 +4828,23 @@
       <c r="B21" s="5">
         <v>16</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="18">
         <v>2</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
@@ -4913,23 +4914,23 @@
       <c r="B22" s="5">
         <v>17</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="18">
         <v>2</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
@@ -4999,23 +5000,23 @@
       <c r="B23" s="5">
         <v>18</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="18">
         <v>2</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
       <c r="P23" s="11"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="11"/>
@@ -5085,23 +5086,23 @@
       <c r="B24" s="5">
         <v>19</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="18">
         <v>2</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
@@ -5171,7 +5172,7 @@
       <c r="B25" s="5">
         <v>20</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="15" t="s">
         <v>95</v>
       </c>
       <c r="D25" s="12">
@@ -5257,10 +5258,10 @@
       <c r="B26" s="5">
         <v>21</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="13">
         <v>1</v>
       </c>
       <c r="E26" s="1"/>
@@ -5352,7 +5353,7 @@
       <c r="C27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="13">
         <v>1</v>
       </c>
       <c r="E27" s="1"/>
@@ -5437,23 +5438,25 @@
       <c r="B28" s="5">
         <v>23</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="13">
         <v>1</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1">
+        <v>1</v>
+      </c>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
       <c r="R28" s="11"/>
@@ -8852,10 +8855,10 @@
       <c r="CA68" s="11"/>
     </row>
     <row r="69" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B69" s="23" t="s">
+      <c r="B69" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="23"/>
+      <c r="C69" s="22"/>
       <c r="D69" s="6">
         <f>SUM(D6:D68)</f>
         <v>63</v>
@@ -8902,270 +8905,270 @@
       </c>
       <c r="O69" s="7">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="P69" s="7">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="Q69" s="7">
         <f t="shared" ref="Q69:AV69" si="1">P69-SUM(Q6:Q68)</f>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="R69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="S69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="T69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="U69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="V69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="W69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="X69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="Y69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>48.5</v>
       </c>
     </row>
     <row r="70" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C70" s="22"/>
+      <c r="C70" s="21"/>
       <c r="D70" s="3">
         <f>SUM(D6:D68)</f>
         <v>63</v>

</xml_diff>

<commit_message>
Big update. Login fixed of typo's
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA797C9-F0DA-4C6A-95F8-03DF546BF727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF7020C-BBDB-4859-AC73-FE58A38AF6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -281,9 +281,6 @@
     <t>MySQL Database</t>
   </si>
   <si>
-    <t>Formulier Velden</t>
-  </si>
-  <si>
     <t>GPS-Locatie Map</t>
   </si>
   <si>
@@ -351,6 +348,21 @@
   </si>
   <si>
     <t>Favicon</t>
+  </si>
+  <si>
+    <t>Makkelijk Ontwerp</t>
+  </si>
+  <si>
+    <t>Gebruikersnaam</t>
+  </si>
+  <si>
+    <t>Inlog Formulier</t>
+  </si>
+  <si>
+    <t>Registreer Formulier</t>
+  </si>
+  <si>
+    <t>Klachten Formulier</t>
   </si>
 </sst>
 </file>
@@ -978,211 +990,211 @@
                   <c:v>59.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57.7</c:v>
+                  <c:v>56.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>48.5</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>48.5</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2531,16 +2543,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>32384</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>166370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2867,20 +2879,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:79" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:79" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
@@ -2962,7 +2974,7 @@
       <c r="BZ2" s="20"/>
       <c r="CA2" s="20"/>
     </row>
-    <row r="3" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -3042,7 +3054,7 @@
       <c r="BZ3" s="20"/>
       <c r="CA3" s="20"/>
     </row>
-    <row r="4" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
@@ -3050,7 +3062,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="9">
         <v>45243</v>
@@ -3278,7 +3290,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="5" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
       <c r="D5" s="8" t="s">
@@ -3510,7 +3522,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -3600,30 +3612,32 @@
       <c r="BZ6" s="11"/>
       <c r="CA6" s="11"/>
     </row>
-    <row r="7" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="18">
+      <c r="C7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="13">
         <v>2</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1">
         <v>0.5</v>
       </c>
-      <c r="P7" s="19"/>
+      <c r="P7" s="1">
+        <v>1.5</v>
+      </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
@@ -3688,7 +3702,7 @@
       <c r="BZ7" s="11"/>
       <c r="CA7" s="11"/>
     </row>
-    <row r="8" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>3</v>
       </c>
@@ -3776,12 +3790,12 @@
       <c r="BZ8" s="11"/>
       <c r="CA8" s="11"/>
     </row>
-    <row r="9" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>4</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="13">
         <v>1</v>
@@ -3864,12 +3878,12 @@
       <c r="BZ9" s="11"/>
       <c r="CA9" s="11"/>
     </row>
-    <row r="10" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>5</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="13">
         <v>0.5</v>
@@ -3952,12 +3966,12 @@
       <c r="BZ10" s="11"/>
       <c r="CA10" s="11"/>
     </row>
-    <row r="11" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>6</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="D11" s="13">
         <v>0.5</v>
@@ -3969,13 +3983,13 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1">
         <v>0.5</v>
       </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
@@ -4040,12 +4054,12 @@
       <c r="BZ11" s="11"/>
       <c r="CA11" s="11"/>
     </row>
-    <row r="12" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>7</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" s="18">
         <v>4</v>
@@ -4128,15 +4142,15 @@
       <c r="BZ12" s="11"/>
       <c r="CA12" s="11"/>
     </row>
-    <row r="13" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>8</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -4145,7 +4159,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
@@ -4216,15 +4230,15 @@
       <c r="BZ13" s="11"/>
       <c r="CA13" s="11"/>
     </row>
-    <row r="14" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>9</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4237,7 +4251,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
@@ -4304,12 +4318,12 @@
       <c r="BZ14" s="11"/>
       <c r="CA14" s="11"/>
     </row>
-    <row r="15" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>10</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="13">
         <v>2</v>
@@ -4392,28 +4406,30 @@
       <c r="BZ15" s="11"/>
       <c r="CA15" s="11"/>
     </row>
-    <row r="16" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>11</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="C16" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="13">
         <v>2</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1">
+        <v>2</v>
+      </c>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
@@ -4478,12 +4494,12 @@
       <c r="BZ16" s="11"/>
       <c r="CA16" s="11"/>
     </row>
-    <row r="17" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>12</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="12">
         <v>2</v>
@@ -4564,12 +4580,12 @@
       <c r="BZ17" s="11"/>
       <c r="CA17" s="11"/>
     </row>
-    <row r="18" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>13</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="12">
         <v>2</v>
@@ -4650,28 +4666,30 @@
       <c r="BZ18" s="11"/>
       <c r="CA18" s="11"/>
     </row>
-    <row r="19" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>14</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="18">
+      <c r="C19" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="13">
         <v>2</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1">
+        <v>2</v>
+      </c>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
@@ -4736,12 +4754,12 @@
       <c r="BZ19" s="11"/>
       <c r="CA19" s="11"/>
     </row>
-    <row r="20" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>15</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="13">
         <v>1</v>
@@ -4824,12 +4842,12 @@
       <c r="BZ20" s="11"/>
       <c r="CA20" s="11"/>
     </row>
-    <row r="21" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>16</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="18">
         <v>2</v>
@@ -4910,12 +4928,12 @@
       <c r="BZ21" s="11"/>
       <c r="CA21" s="11"/>
     </row>
-    <row r="22" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>17</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="18">
         <v>2</v>
@@ -4996,12 +5014,12 @@
       <c r="BZ22" s="11"/>
       <c r="CA22" s="11"/>
     </row>
-    <row r="23" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>18</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="18">
         <v>2</v>
@@ -5082,12 +5100,12 @@
       <c r="BZ23" s="11"/>
       <c r="CA23" s="11"/>
     </row>
-    <row r="24" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>19</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="18">
         <v>2</v>
@@ -5168,12 +5186,12 @@
       <c r="BZ24" s="11"/>
       <c r="CA24" s="11"/>
     </row>
-    <row r="25" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
         <v>20</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D25" s="12">
         <v>2</v>
@@ -5254,12 +5272,12 @@
       <c r="BZ25" s="11"/>
       <c r="CA25" s="11"/>
     </row>
-    <row r="26" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>21</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D26" s="13">
         <v>1</v>
@@ -5346,12 +5364,12 @@
       <c r="BZ26" s="11"/>
       <c r="CA26" s="11"/>
     </row>
-    <row r="27" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="13">
         <v>1</v>
@@ -5434,12 +5452,12 @@
       <c r="BZ27" s="11"/>
       <c r="CA27" s="11"/>
     </row>
-    <row r="28" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>23</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="13">
         <v>1</v>
@@ -5522,26 +5540,30 @@
       <c r="BZ28" s="11"/>
       <c r="CA28" s="11"/>
     </row>
-    <row r="29" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
         <v>24</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12">
+      <c r="C29" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="13">
         <v>1</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1">
+        <v>1</v>
+      </c>
       <c r="Q29" s="11"/>
       <c r="R29" s="11"/>
       <c r="S29" s="11"/>
@@ -5606,26 +5628,30 @@
       <c r="BZ29" s="11"/>
       <c r="CA29" s="11"/>
     </row>
-    <row r="30" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B30" s="5">
         <v>25</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12">
+      <c r="C30" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="13">
         <v>1</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13">
+        <v>1</v>
+      </c>
       <c r="Q30" s="11"/>
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
@@ -5690,26 +5716,30 @@
       <c r="BZ30" s="11"/>
       <c r="CA30" s="11"/>
     </row>
-    <row r="31" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B31" s="5">
         <v>26</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12">
+      <c r="C31" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="13">
         <v>1</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13">
+        <v>1</v>
+      </c>
       <c r="Q31" s="11"/>
       <c r="R31" s="11"/>
       <c r="S31" s="11"/>
@@ -5774,26 +5804,30 @@
       <c r="BZ31" s="11"/>
       <c r="CA31" s="11"/>
     </row>
-    <row r="32" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B32" s="5">
         <v>27</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12">
+      <c r="C32" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="13">
         <v>1</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13">
+        <v>1</v>
+      </c>
       <c r="Q32" s="11"/>
       <c r="R32" s="11"/>
       <c r="S32" s="11"/>
@@ -5858,7 +5892,7 @@
       <c r="BZ32" s="11"/>
       <c r="CA32" s="11"/>
     </row>
-    <row r="33" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B33" s="5">
         <v>28</v>
       </c>
@@ -5942,7 +5976,7 @@
       <c r="BZ33" s="11"/>
       <c r="CA33" s="11"/>
     </row>
-    <row r="34" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B34" s="5">
         <v>29</v>
       </c>
@@ -6026,7 +6060,7 @@
       <c r="BZ34" s="11"/>
       <c r="CA34" s="11"/>
     </row>
-    <row r="35" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B35" s="5">
         <v>30</v>
       </c>
@@ -6110,7 +6144,7 @@
       <c r="BZ35" s="11"/>
       <c r="CA35" s="11"/>
     </row>
-    <row r="36" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B36" s="5">
         <v>31</v>
       </c>
@@ -6194,7 +6228,7 @@
       <c r="BZ36" s="11"/>
       <c r="CA36" s="11"/>
     </row>
-    <row r="37" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B37" s="5">
         <v>32</v>
       </c>
@@ -6278,7 +6312,7 @@
       <c r="BZ37" s="11"/>
       <c r="CA37" s="11"/>
     </row>
-    <row r="38" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B38" s="5">
         <v>33</v>
       </c>
@@ -6362,7 +6396,7 @@
       <c r="BZ38" s="11"/>
       <c r="CA38" s="11"/>
     </row>
-    <row r="39" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B39" s="5">
         <v>34</v>
       </c>
@@ -6446,7 +6480,7 @@
       <c r="BZ39" s="11"/>
       <c r="CA39" s="11"/>
     </row>
-    <row r="40" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B40" s="5">
         <v>35</v>
       </c>
@@ -6530,7 +6564,7 @@
       <c r="BZ40" s="11"/>
       <c r="CA40" s="11"/>
     </row>
-    <row r="41" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B41" s="5">
         <v>36</v>
       </c>
@@ -6614,7 +6648,7 @@
       <c r="BZ41" s="11"/>
       <c r="CA41" s="11"/>
     </row>
-    <row r="42" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B42" s="5">
         <v>37</v>
       </c>
@@ -6698,7 +6732,7 @@
       <c r="BZ42" s="11"/>
       <c r="CA42" s="11"/>
     </row>
-    <row r="43" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B43" s="5">
         <v>38</v>
       </c>
@@ -6782,7 +6816,7 @@
       <c r="BZ43" s="11"/>
       <c r="CA43" s="11"/>
     </row>
-    <row r="44" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B44" s="5">
         <v>39</v>
       </c>
@@ -6866,7 +6900,7 @@
       <c r="BZ44" s="11"/>
       <c r="CA44" s="11"/>
     </row>
-    <row r="45" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B45" s="5">
         <v>40</v>
       </c>
@@ -6950,7 +6984,7 @@
       <c r="BZ45" s="11"/>
       <c r="CA45" s="11"/>
     </row>
-    <row r="46" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B46" s="5">
         <v>41</v>
       </c>
@@ -7034,7 +7068,7 @@
       <c r="BZ46" s="11"/>
       <c r="CA46" s="11"/>
     </row>
-    <row r="47" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B47" s="5">
         <v>42</v>
       </c>
@@ -7118,7 +7152,7 @@
       <c r="BZ47" s="11"/>
       <c r="CA47" s="11"/>
     </row>
-    <row r="48" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B48" s="5">
         <v>43</v>
       </c>
@@ -7202,7 +7236,7 @@
       <c r="BZ48" s="11"/>
       <c r="CA48" s="11"/>
     </row>
-    <row r="49" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B49" s="5">
         <v>44</v>
       </c>
@@ -7286,7 +7320,7 @@
       <c r="BZ49" s="11"/>
       <c r="CA49" s="11"/>
     </row>
-    <row r="50" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B50" s="5">
         <v>45</v>
       </c>
@@ -7370,14 +7404,12 @@
       <c r="BZ50" s="11"/>
       <c r="CA50" s="11"/>
     </row>
-    <row r="51" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B51" s="5">
         <v>46</v>
       </c>
       <c r="C51" s="11"/>
-      <c r="D51" s="12">
-        <v>1</v>
-      </c>
+      <c r="D51" s="12"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -7454,14 +7486,12 @@
       <c r="BZ51" s="11"/>
       <c r="CA51" s="11"/>
     </row>
-    <row r="52" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B52" s="5">
         <v>47</v>
       </c>
       <c r="C52" s="11"/>
-      <c r="D52" s="12">
-        <v>1</v>
-      </c>
+      <c r="D52" s="12"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
@@ -7538,14 +7568,12 @@
       <c r="BZ52" s="11"/>
       <c r="CA52" s="11"/>
     </row>
-    <row r="53" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B53" s="5">
         <v>48</v>
       </c>
       <c r="C53" s="11"/>
-      <c r="D53" s="12">
-        <v>1</v>
-      </c>
+      <c r="D53" s="12"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
@@ -7622,14 +7650,12 @@
       <c r="BZ53" s="11"/>
       <c r="CA53" s="11"/>
     </row>
-    <row r="54" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B54" s="5">
         <v>49</v>
       </c>
       <c r="C54" s="11"/>
-      <c r="D54" s="12">
-        <v>1</v>
-      </c>
+      <c r="D54" s="12"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
@@ -7706,7 +7732,7 @@
       <c r="BZ54" s="11"/>
       <c r="CA54" s="11"/>
     </row>
-    <row r="55" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B55" s="5">
         <v>50</v>
       </c>
@@ -7788,7 +7814,7 @@
       <c r="BZ55" s="11"/>
       <c r="CA55" s="11"/>
     </row>
-    <row r="56" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B56" s="5">
         <v>51</v>
       </c>
@@ -7870,7 +7896,7 @@
       <c r="BZ56" s="11"/>
       <c r="CA56" s="11"/>
     </row>
-    <row r="57" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B57" s="5">
         <v>52</v>
       </c>
@@ -7952,7 +7978,7 @@
       <c r="BZ57" s="11"/>
       <c r="CA57" s="11"/>
     </row>
-    <row r="58" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B58" s="5">
         <v>53</v>
       </c>
@@ -8034,7 +8060,7 @@
       <c r="BZ58" s="11"/>
       <c r="CA58" s="11"/>
     </row>
-    <row r="59" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B59" s="5">
         <v>54</v>
       </c>
@@ -8116,7 +8142,7 @@
       <c r="BZ59" s="11"/>
       <c r="CA59" s="11"/>
     </row>
-    <row r="60" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B60" s="5">
         <v>55</v>
       </c>
@@ -8198,7 +8224,7 @@
       <c r="BZ60" s="11"/>
       <c r="CA60" s="11"/>
     </row>
-    <row r="61" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B61" s="5">
         <v>56</v>
       </c>
@@ -8280,7 +8306,7 @@
       <c r="BZ61" s="11"/>
       <c r="CA61" s="11"/>
     </row>
-    <row r="62" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B62" s="5">
         <v>57</v>
       </c>
@@ -8362,7 +8388,7 @@
       <c r="BZ62" s="11"/>
       <c r="CA62" s="11"/>
     </row>
-    <row r="63" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B63" s="5">
         <v>58</v>
       </c>
@@ -8444,7 +8470,7 @@
       <c r="BZ63" s="11"/>
       <c r="CA63" s="11"/>
     </row>
-    <row r="64" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B64" s="5">
         <v>59</v>
       </c>
@@ -8526,7 +8552,7 @@
       <c r="BZ64" s="11"/>
       <c r="CA64" s="11"/>
     </row>
-    <row r="65" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B65" s="5">
         <v>60</v>
       </c>
@@ -8608,7 +8634,7 @@
       <c r="BZ65" s="11"/>
       <c r="CA65" s="11"/>
     </row>
-    <row r="66" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B66" s="5">
         <v>61</v>
       </c>
@@ -8690,7 +8716,7 @@
       <c r="BZ66" s="11"/>
       <c r="CA66" s="11"/>
     </row>
-    <row r="67" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B67" s="5">
         <v>62</v>
       </c>
@@ -8772,7 +8798,7 @@
       <c r="BZ67" s="11"/>
       <c r="CA67" s="11"/>
     </row>
-    <row r="68" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B68" s="5">
         <v>63</v>
       </c>
@@ -8854,9 +8880,9 @@
       <c r="BZ68" s="11"/>
       <c r="CA68" s="11"/>
     </row>
-    <row r="69" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B69" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C69" s="22"/>
       <c r="D69" s="6">
@@ -8889,284 +8915,284 @@
       </c>
       <c r="K69" s="7">
         <f t="shared" si="0"/>
-        <v>57.7</v>
+        <v>56.7</v>
       </c>
       <c r="L69" s="7">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>52.5</v>
       </c>
       <c r="M69" s="7">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>52.5</v>
       </c>
       <c r="N69" s="7">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>52.5</v>
       </c>
       <c r="O69" s="7">
         <f t="shared" si="0"/>
-        <v>48.5</v>
+        <v>45</v>
       </c>
       <c r="P69" s="7">
         <f t="shared" si="0"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="Q69" s="7">
         <f t="shared" ref="Q69:AV69" si="1">P69-SUM(Q6:Q68)</f>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="R69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="S69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="T69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="U69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="V69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="W69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="X69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="Y69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>48.5</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="70" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B70" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C70" s="21"/>
       <c r="D70" s="3">

</xml_diff>

<commit_message>
Map, klachten php crud+search klaar, docs update
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF7020C-BBDB-4859-AC73-FE58A38AF6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6220C0C-EE8C-4DD2-AEA0-FB445C53C13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -363,6 +363,12 @@
   </si>
   <si>
     <t>Klachten Formulier</t>
+  </si>
+  <si>
+    <t>Gegevens meesturen</t>
+  </si>
+  <si>
+    <t>Admin Interface</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,12 +489,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -521,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -561,19 +561,16 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -993,208 +990,208 @@
                   <c:v>56.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>52.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>35</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,8 +2876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2893,172 +2890,172 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:79" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="20"/>
-      <c r="BA2" s="20"/>
-      <c r="BB2" s="20"/>
-      <c r="BC2" s="20"/>
-      <c r="BD2" s="20"/>
-      <c r="BE2" s="20"/>
-      <c r="BF2" s="20"/>
-      <c r="BG2" s="20"/>
-      <c r="BH2" s="20"/>
-      <c r="BI2" s="20"/>
-      <c r="BJ2" s="20"/>
-      <c r="BK2" s="20"/>
-      <c r="BL2" s="20"/>
-      <c r="BM2" s="20"/>
-      <c r="BN2" s="20"/>
-      <c r="BO2" s="20"/>
-      <c r="BP2" s="20"/>
-      <c r="BQ2" s="20"/>
-      <c r="BR2" s="20"/>
-      <c r="BS2" s="20"/>
-      <c r="BT2" s="20"/>
-      <c r="BU2" s="20"/>
-      <c r="BV2" s="20"/>
-      <c r="BW2" s="20"/>
-      <c r="BX2" s="20"/>
-      <c r="BY2" s="20"/>
-      <c r="BZ2" s="20"/>
-      <c r="CA2" s="20"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="19"/>
+      <c r="AQ2" s="19"/>
+      <c r="AR2" s="19"/>
+      <c r="AS2" s="19"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="19"/>
+      <c r="BH2" s="19"/>
+      <c r="BI2" s="19"/>
+      <c r="BJ2" s="19"/>
+      <c r="BK2" s="19"/>
+      <c r="BL2" s="19"/>
+      <c r="BM2" s="19"/>
+      <c r="BN2" s="19"/>
+      <c r="BO2" s="19"/>
+      <c r="BP2" s="19"/>
+      <c r="BQ2" s="19"/>
+      <c r="BR2" s="19"/>
+      <c r="BS2" s="19"/>
+      <c r="BT2" s="19"/>
+      <c r="BU2" s="19"/>
+      <c r="BV2" s="19"/>
+      <c r="BW2" s="19"/>
+      <c r="BX2" s="19"/>
+      <c r="BY2" s="19"/>
+      <c r="BZ2" s="19"/>
+      <c r="CA2" s="19"/>
     </row>
     <row r="3" spans="2:79" x14ac:dyDescent="0.3">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="20"/>
-      <c r="AK3" s="20"/>
-      <c r="AL3" s="20"/>
-      <c r="AM3" s="20"/>
-      <c r="AN3" s="20"/>
-      <c r="AO3" s="20"/>
-      <c r="AP3" s="20"/>
-      <c r="AQ3" s="20"/>
-      <c r="AR3" s="20"/>
-      <c r="AS3" s="20"/>
-      <c r="AT3" s="20"/>
-      <c r="AU3" s="20"/>
-      <c r="AV3" s="20"/>
-      <c r="AW3" s="20"/>
-      <c r="AX3" s="20"/>
-      <c r="AY3" s="20"/>
-      <c r="AZ3" s="20"/>
-      <c r="BA3" s="20"/>
-      <c r="BB3" s="20"/>
-      <c r="BC3" s="20"/>
-      <c r="BD3" s="20"/>
-      <c r="BE3" s="20"/>
-      <c r="BF3" s="20"/>
-      <c r="BG3" s="20"/>
-      <c r="BH3" s="20"/>
-      <c r="BI3" s="20"/>
-      <c r="BJ3" s="20"/>
-      <c r="BK3" s="20"/>
-      <c r="BL3" s="20"/>
-      <c r="BM3" s="20"/>
-      <c r="BN3" s="20"/>
-      <c r="BO3" s="20"/>
-      <c r="BP3" s="20"/>
-      <c r="BQ3" s="20"/>
-      <c r="BR3" s="20"/>
-      <c r="BS3" s="20"/>
-      <c r="BT3" s="20"/>
-      <c r="BU3" s="20"/>
-      <c r="BV3" s="20"/>
-      <c r="BW3" s="20"/>
-      <c r="BX3" s="20"/>
-      <c r="BY3" s="20"/>
-      <c r="BZ3" s="20"/>
-      <c r="CA3" s="20"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="19"/>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="19"/>
+      <c r="AL3" s="19"/>
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="19"/>
+      <c r="AR3" s="19"/>
+      <c r="AS3" s="19"/>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="19"/>
+      <c r="AW3" s="19"/>
+      <c r="AX3" s="19"/>
+      <c r="AY3" s="19"/>
+      <c r="AZ3" s="19"/>
+      <c r="BA3" s="19"/>
+      <c r="BB3" s="19"/>
+      <c r="BC3" s="19"/>
+      <c r="BD3" s="19"/>
+      <c r="BE3" s="19"/>
+      <c r="BF3" s="19"/>
+      <c r="BG3" s="19"/>
+      <c r="BH3" s="19"/>
+      <c r="BI3" s="19"/>
+      <c r="BJ3" s="19"/>
+      <c r="BK3" s="19"/>
+      <c r="BL3" s="19"/>
+      <c r="BM3" s="19"/>
+      <c r="BN3" s="19"/>
+      <c r="BO3" s="19"/>
+      <c r="BP3" s="19"/>
+      <c r="BQ3" s="19"/>
+      <c r="BR3" s="19"/>
+      <c r="BS3" s="19"/>
+      <c r="BT3" s="19"/>
+      <c r="BU3" s="19"/>
+      <c r="BV3" s="19"/>
+      <c r="BW3" s="19"/>
+      <c r="BX3" s="19"/>
+      <c r="BY3" s="19"/>
+      <c r="BZ3" s="19"/>
+      <c r="CA3" s="19"/>
     </row>
     <row r="4" spans="2:79" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -3291,8 +3288,8 @@
       </c>
     </row>
     <row r="5" spans="2:79" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
@@ -3526,7 +3523,7 @@
       <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>79</v>
       </c>
       <c r="D6" s="13">
@@ -3616,7 +3613,7 @@
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>82</v>
       </c>
       <c r="D7" s="13">
@@ -3794,7 +3791,7 @@
       <c r="B9" s="5">
         <v>4</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>101</v>
       </c>
       <c r="D9" s="13">
@@ -3882,7 +3879,7 @@
       <c r="B10" s="5">
         <v>5</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>102</v>
       </c>
       <c r="D10" s="13">
@@ -3970,7 +3967,7 @@
       <c r="B11" s="5">
         <v>6</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>105</v>
       </c>
       <c r="D11" s="13">
@@ -4058,27 +4055,29 @@
       <c r="B12" s="5">
         <v>7</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="17">
         <v>4</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19">
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18">
         <v>1</v>
       </c>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="11"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18">
+        <v>3</v>
+      </c>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
       <c r="T12" s="11"/>
@@ -4146,7 +4145,7 @@
       <c r="B13" s="5">
         <v>8</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>83</v>
       </c>
       <c r="D13" s="13">
@@ -4234,7 +4233,7 @@
       <c r="B14" s="5">
         <v>9</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>84</v>
       </c>
       <c r="D14" s="13">
@@ -4322,7 +4321,7 @@
       <c r="B15" s="5">
         <v>10</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="13">
@@ -4410,7 +4409,7 @@
       <c r="B16" s="5">
         <v>11</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>86</v>
       </c>
       <c r="D16" s="13">
@@ -4670,7 +4669,7 @@
       <c r="B19" s="5">
         <v>14</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>89</v>
       </c>
       <c r="D19" s="13">
@@ -4758,7 +4757,7 @@
       <c r="B20" s="5">
         <v>15</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>95</v>
       </c>
       <c r="D20" s="13">
@@ -4846,25 +4845,27 @@
       <c r="B21" s="5">
         <v>16</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="13">
         <v>2</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="1">
+        <v>2</v>
+      </c>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
@@ -4932,25 +4933,27 @@
       <c r="B22" s="5">
         <v>17</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="13">
         <v>2</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="1">
+        <v>2</v>
+      </c>
       <c r="R22" s="11"/>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
@@ -5018,25 +5021,27 @@
       <c r="B23" s="5">
         <v>18</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="13">
         <v>2</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="1">
+        <v>2</v>
+      </c>
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
@@ -5104,25 +5109,27 @@
       <c r="B24" s="5">
         <v>19</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="13">
         <v>2</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="1">
+        <v>2</v>
+      </c>
       <c r="R24" s="11"/>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
@@ -5193,7 +5200,7 @@
       <c r="C25" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="13">
         <v>2</v>
       </c>
       <c r="E25" s="11"/>
@@ -5208,7 +5215,9 @@
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
+      <c r="Q25" s="1">
+        <v>2</v>
+      </c>
       <c r="R25" s="11"/>
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
@@ -5276,7 +5285,7 @@
       <c r="B26" s="5">
         <v>21</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D26" s="13">
@@ -5456,7 +5465,7 @@
       <c r="B28" s="5">
         <v>23</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>103</v>
       </c>
       <c r="D28" s="13">
@@ -5544,7 +5553,7 @@
       <c r="B29" s="5">
         <v>24</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>104</v>
       </c>
       <c r="D29" s="13">
@@ -5632,7 +5641,7 @@
       <c r="B30" s="5">
         <v>25</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="15" t="s">
         <v>106</v>
       </c>
       <c r="D30" s="13">
@@ -5720,7 +5729,7 @@
       <c r="B31" s="5">
         <v>26</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="15" t="s">
         <v>107</v>
       </c>
       <c r="D31" s="13">
@@ -5808,7 +5817,7 @@
       <c r="B32" s="5">
         <v>27</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="15" t="s">
         <v>108</v>
       </c>
       <c r="D32" s="13">
@@ -5896,18 +5905,22 @@
       <c r="B33" s="5">
         <v>28</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12">
+      <c r="C33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="13">
         <v>1</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
       <c r="M33" s="11"/>
       <c r="N33" s="11"/>
       <c r="O33" s="11"/>
@@ -5980,23 +5993,27 @@
       <c r="B34" s="5">
         <v>29</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12">
+      <c r="C34" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="17">
+        <v>2</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18">
         <v>1</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
       <c r="R34" s="11"/>
       <c r="S34" s="11"/>
       <c r="T34" s="11"/>
@@ -7325,9 +7342,7 @@
         <v>45</v>
       </c>
       <c r="C50" s="11"/>
-      <c r="D50" s="12">
-        <v>1</v>
-      </c>
+      <c r="D50" s="12"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
@@ -8881,10 +8896,10 @@
       <c r="CA68" s="11"/>
     </row>
     <row r="69" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="22"/>
+      <c r="C69" s="21"/>
       <c r="D69" s="6">
         <f>SUM(D6:D68)</f>
         <v>63</v>
@@ -8919,282 +8934,282 @@
       </c>
       <c r="L69" s="7">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>50.5</v>
       </c>
       <c r="M69" s="7">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>50.5</v>
       </c>
       <c r="N69" s="7">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>50.5</v>
       </c>
       <c r="O69" s="7">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="P69" s="7">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q69" s="7">
         <f t="shared" ref="Q69:AV69" si="1">P69-SUM(Q6:Q68)</f>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="S69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="T69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="U69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="V69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="W69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="X69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="Y69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B70" s="21" t="s">
+      <c r="B70" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="21"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="3">
         <f>SUM(D6:D68)</f>
         <v>63</v>

</xml_diff>

<commit_message>
Fix for proper saving coordinates, complaint form update
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45980925-B9AB-4E72-862A-9AAA8EDFB6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516F57EF-2746-4219-A1B9-F5C0808D2740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -617,8 +617,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF99"/>
       <color rgb="FF9999FF"/>
-      <color rgb="FF99FF99"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFFFF99"/>
@@ -1035,7 +1035,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>20</c:v>
@@ -2897,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J18" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4101,8 +4101,12 @@
       </c>
       <c r="R12" s="18"/>
       <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="11"/>
+      <c r="T12" s="18">
+        <v>-1</v>
+      </c>
+      <c r="U12" s="18">
+        <v>1</v>
+      </c>
       <c r="V12" s="11"/>
       <c r="W12" s="11"/>
       <c r="X12" s="11"/>
@@ -4889,8 +4893,12 @@
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
+      <c r="T21" s="18">
+        <v>-1</v>
+      </c>
+      <c r="U21" s="1">
+        <v>1</v>
+      </c>
       <c r="V21" s="11"/>
       <c r="W21" s="11"/>
       <c r="X21" s="11"/>
@@ -5065,8 +5073,12 @@
       </c>
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
+      <c r="T23" s="18">
+        <v>-1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>1</v>
+      </c>
       <c r="V23" s="11"/>
       <c r="W23" s="11"/>
       <c r="X23" s="11"/>
@@ -8979,7 +8991,7 @@
       </c>
       <c r="T69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="U69" s="7">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Update on gps map, navbar, docs
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516F57EF-2746-4219-A1B9-F5C0808D2740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD343DA1-F24D-4CE7-8E5E-7CF6993764E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -365,9 +365,6 @@
     <t>Klachten Formulier</t>
   </si>
   <si>
-    <t>Gegevens meesturen</t>
-  </si>
-  <si>
     <t>Admin Interface</t>
   </si>
   <si>
@@ -381,6 +378,21 @@
   </si>
   <si>
     <t>Zoekfilters</t>
+  </si>
+  <si>
+    <t>Gegevens sturen PHP</t>
+  </si>
+  <si>
+    <t>Use Case Diagram</t>
+  </si>
+  <si>
+    <t>ERD</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
   </si>
 </sst>
 </file>
@@ -462,7 +474,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +520,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,9 +601,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -608,6 +623,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,178 +1059,178 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2898,185 +2916,185 @@
   <dimension ref="B2:CA70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:79" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:79" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="20"/>
-      <c r="BA2" s="20"/>
-      <c r="BB2" s="20"/>
-      <c r="BC2" s="20"/>
-      <c r="BD2" s="20"/>
-      <c r="BE2" s="20"/>
-      <c r="BF2" s="20"/>
-      <c r="BG2" s="20"/>
-      <c r="BH2" s="20"/>
-      <c r="BI2" s="20"/>
-      <c r="BJ2" s="20"/>
-      <c r="BK2" s="20"/>
-      <c r="BL2" s="20"/>
-      <c r="BM2" s="20"/>
-      <c r="BN2" s="20"/>
-      <c r="BO2" s="20"/>
-      <c r="BP2" s="20"/>
-      <c r="BQ2" s="20"/>
-      <c r="BR2" s="20"/>
-      <c r="BS2" s="20"/>
-      <c r="BT2" s="20"/>
-      <c r="BU2" s="20"/>
-      <c r="BV2" s="20"/>
-      <c r="BW2" s="20"/>
-      <c r="BX2" s="20"/>
-      <c r="BY2" s="20"/>
-      <c r="BZ2" s="20"/>
-      <c r="CA2" s="20"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="19"/>
+      <c r="AP2" s="19"/>
+      <c r="AQ2" s="19"/>
+      <c r="AR2" s="19"/>
+      <c r="AS2" s="19"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="19"/>
+      <c r="BC2" s="19"/>
+      <c r="BD2" s="19"/>
+      <c r="BE2" s="19"/>
+      <c r="BF2" s="19"/>
+      <c r="BG2" s="19"/>
+      <c r="BH2" s="19"/>
+      <c r="BI2" s="19"/>
+      <c r="BJ2" s="19"/>
+      <c r="BK2" s="19"/>
+      <c r="BL2" s="19"/>
+      <c r="BM2" s="19"/>
+      <c r="BN2" s="19"/>
+      <c r="BO2" s="19"/>
+      <c r="BP2" s="19"/>
+      <c r="BQ2" s="19"/>
+      <c r="BR2" s="19"/>
+      <c r="BS2" s="19"/>
+      <c r="BT2" s="19"/>
+      <c r="BU2" s="19"/>
+      <c r="BV2" s="19"/>
+      <c r="BW2" s="19"/>
+      <c r="BX2" s="19"/>
+      <c r="BY2" s="19"/>
+      <c r="BZ2" s="19"/>
+      <c r="CA2" s="19"/>
     </row>
-    <row r="3" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
-      <c r="AA3" s="20"/>
-      <c r="AB3" s="20"/>
-      <c r="AC3" s="20"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="20"/>
-      <c r="AF3" s="20"/>
-      <c r="AG3" s="20"/>
-      <c r="AH3" s="20"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="20"/>
-      <c r="AK3" s="20"/>
-      <c r="AL3" s="20"/>
-      <c r="AM3" s="20"/>
-      <c r="AN3" s="20"/>
-      <c r="AO3" s="20"/>
-      <c r="AP3" s="20"/>
-      <c r="AQ3" s="20"/>
-      <c r="AR3" s="20"/>
-      <c r="AS3" s="20"/>
-      <c r="AT3" s="20"/>
-      <c r="AU3" s="20"/>
-      <c r="AV3" s="20"/>
-      <c r="AW3" s="20"/>
-      <c r="AX3" s="20"/>
-      <c r="AY3" s="20"/>
-      <c r="AZ3" s="20"/>
-      <c r="BA3" s="20"/>
-      <c r="BB3" s="20"/>
-      <c r="BC3" s="20"/>
-      <c r="BD3" s="20"/>
-      <c r="BE3" s="20"/>
-      <c r="BF3" s="20"/>
-      <c r="BG3" s="20"/>
-      <c r="BH3" s="20"/>
-      <c r="BI3" s="20"/>
-      <c r="BJ3" s="20"/>
-      <c r="BK3" s="20"/>
-      <c r="BL3" s="20"/>
-      <c r="BM3" s="20"/>
-      <c r="BN3" s="20"/>
-      <c r="BO3" s="20"/>
-      <c r="BP3" s="20"/>
-      <c r="BQ3" s="20"/>
-      <c r="BR3" s="20"/>
-      <c r="BS3" s="20"/>
-      <c r="BT3" s="20"/>
-      <c r="BU3" s="20"/>
-      <c r="BV3" s="20"/>
-      <c r="BW3" s="20"/>
-      <c r="BX3" s="20"/>
-      <c r="BY3" s="20"/>
-      <c r="BZ3" s="20"/>
-      <c r="CA3" s="20"/>
+    <row r="3" spans="2:79" x14ac:dyDescent="0.3">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="19"/>
+      <c r="AJ3" s="19"/>
+      <c r="AK3" s="19"/>
+      <c r="AL3" s="19"/>
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="19"/>
+      <c r="AQ3" s="19"/>
+      <c r="AR3" s="19"/>
+      <c r="AS3" s="19"/>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="19"/>
+      <c r="AW3" s="19"/>
+      <c r="AX3" s="19"/>
+      <c r="AY3" s="19"/>
+      <c r="AZ3" s="19"/>
+      <c r="BA3" s="19"/>
+      <c r="BB3" s="19"/>
+      <c r="BC3" s="19"/>
+      <c r="BD3" s="19"/>
+      <c r="BE3" s="19"/>
+      <c r="BF3" s="19"/>
+      <c r="BG3" s="19"/>
+      <c r="BH3" s="19"/>
+      <c r="BI3" s="19"/>
+      <c r="BJ3" s="19"/>
+      <c r="BK3" s="19"/>
+      <c r="BL3" s="19"/>
+      <c r="BM3" s="19"/>
+      <c r="BN3" s="19"/>
+      <c r="BO3" s="19"/>
+      <c r="BP3" s="19"/>
+      <c r="BQ3" s="19"/>
+      <c r="BR3" s="19"/>
+      <c r="BS3" s="19"/>
+      <c r="BT3" s="19"/>
+      <c r="BU3" s="19"/>
+      <c r="BV3" s="19"/>
+      <c r="BW3" s="19"/>
+      <c r="BX3" s="19"/>
+      <c r="BY3" s="19"/>
+      <c r="BZ3" s="19"/>
+      <c r="CA3" s="19"/>
     </row>
-    <row r="4" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="2:79" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -3308,9 +3326,9 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="5" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+    <row r="5" spans="2:79" x14ac:dyDescent="0.3">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
@@ -3540,7 +3558,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -3630,7 +3648,7 @@
       <c r="BZ6" s="11"/>
       <c r="CA6" s="11"/>
     </row>
-    <row r="7" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>2</v>
       </c>
@@ -3720,7 +3738,7 @@
       <c r="BZ7" s="11"/>
       <c r="CA7" s="11"/>
     </row>
-    <row r="8" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>3</v>
       </c>
@@ -3808,7 +3826,7 @@
       <c r="BZ8" s="11"/>
       <c r="CA8" s="11"/>
     </row>
-    <row r="9" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>4</v>
       </c>
@@ -3896,7 +3914,7 @@
       <c r="BZ9" s="11"/>
       <c r="CA9" s="11"/>
     </row>
-    <row r="10" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>5</v>
       </c>
@@ -3984,7 +4002,7 @@
       <c r="BZ10" s="11"/>
       <c r="CA10" s="11"/>
     </row>
-    <row r="11" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>6</v>
       </c>
@@ -4072,42 +4090,44 @@
       <c r="BZ11" s="11"/>
       <c r="CA11" s="11"/>
     </row>
-    <row r="12" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>7</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="13">
         <v>4</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
         <v>1</v>
       </c>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18">
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1">
         <v>2</v>
       </c>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18">
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1">
         <v>-1</v>
       </c>
-      <c r="U12" s="18">
+      <c r="U12" s="1">
         <v>1</v>
       </c>
-      <c r="V12" s="11"/>
+      <c r="V12" s="1">
+        <v>1</v>
+      </c>
       <c r="W12" s="11"/>
       <c r="X12" s="11"/>
       <c r="Y12" s="11"/>
@@ -4166,7 +4186,7 @@
       <c r="BZ12" s="11"/>
       <c r="CA12" s="11"/>
     </row>
-    <row r="13" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>8</v>
       </c>
@@ -4254,7 +4274,7 @@
       <c r="BZ13" s="11"/>
       <c r="CA13" s="11"/>
     </row>
-    <row r="14" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>9</v>
       </c>
@@ -4342,7 +4362,7 @@
       <c r="BZ14" s="11"/>
       <c r="CA14" s="11"/>
     </row>
-    <row r="15" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>10</v>
       </c>
@@ -4430,7 +4450,7 @@
       <c r="BZ15" s="11"/>
       <c r="CA15" s="11"/>
     </row>
-    <row r="16" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>11</v>
       </c>
@@ -4518,7 +4538,7 @@
       <c r="BZ16" s="11"/>
       <c r="CA16" s="11"/>
     </row>
-    <row r="17" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>12</v>
       </c>
@@ -4604,7 +4624,7 @@
       <c r="BZ17" s="11"/>
       <c r="CA17" s="11"/>
     </row>
-    <row r="18" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>13</v>
       </c>
@@ -4690,7 +4710,7 @@
       <c r="BZ18" s="11"/>
       <c r="CA18" s="11"/>
     </row>
-    <row r="19" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>14</v>
       </c>
@@ -4778,7 +4798,7 @@
       <c r="BZ19" s="11"/>
       <c r="CA19" s="11"/>
     </row>
-    <row r="20" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>15</v>
       </c>
@@ -4866,7 +4886,7 @@
       <c r="BZ20" s="11"/>
       <c r="CA20" s="11"/>
     </row>
-    <row r="21" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>16</v>
       </c>
@@ -4893,7 +4913,7 @@
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
-      <c r="T21" s="18">
+      <c r="T21" s="17">
         <v>-1</v>
       </c>
       <c r="U21" s="1">
@@ -4958,7 +4978,7 @@
       <c r="BZ21" s="11"/>
       <c r="CA21" s="11"/>
     </row>
-    <row r="22" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>17</v>
       </c>
@@ -5046,7 +5066,7 @@
       <c r="BZ22" s="11"/>
       <c r="CA22" s="11"/>
     </row>
-    <row r="23" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>18</v>
       </c>
@@ -5073,7 +5093,7 @@
       </c>
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
-      <c r="T23" s="18">
+      <c r="T23" s="17">
         <v>-1</v>
       </c>
       <c r="U23" s="1">
@@ -5138,7 +5158,7 @@
       <c r="BZ23" s="11"/>
       <c r="CA23" s="11"/>
     </row>
-    <row r="24" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>19</v>
       </c>
@@ -5226,7 +5246,7 @@
       <c r="BZ24" s="11"/>
       <c r="CA24" s="11"/>
     </row>
-    <row r="25" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
         <v>20</v>
       </c>
@@ -5314,7 +5334,7 @@
       <c r="BZ25" s="11"/>
       <c r="CA25" s="11"/>
     </row>
-    <row r="26" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>21</v>
       </c>
@@ -5406,7 +5426,7 @@
       <c r="BZ26" s="11"/>
       <c r="CA26" s="11"/>
     </row>
-    <row r="27" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>22</v>
       </c>
@@ -5494,7 +5514,7 @@
       <c r="BZ27" s="11"/>
       <c r="CA27" s="11"/>
     </row>
-    <row r="28" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>23</v>
       </c>
@@ -5582,7 +5602,7 @@
       <c r="BZ28" s="11"/>
       <c r="CA28" s="11"/>
     </row>
-    <row r="29" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
         <v>24</v>
       </c>
@@ -5670,7 +5690,7 @@
       <c r="BZ29" s="11"/>
       <c r="CA29" s="11"/>
     </row>
-    <row r="30" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B30" s="5">
         <v>25</v>
       </c>
@@ -5758,7 +5778,7 @@
       <c r="BZ30" s="11"/>
       <c r="CA30" s="11"/>
     </row>
-    <row r="31" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B31" s="5">
         <v>26</v>
       </c>
@@ -5846,7 +5866,7 @@
       <c r="BZ31" s="11"/>
       <c r="CA31" s="11"/>
     </row>
-    <row r="32" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B32" s="5">
         <v>27</v>
       </c>
@@ -5934,12 +5954,12 @@
       <c r="BZ32" s="11"/>
       <c r="CA32" s="11"/>
     </row>
-    <row r="33" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B33" s="5">
         <v>28</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>109</v>
+      <c r="C33" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D33" s="13">
         <v>1</v>
@@ -6022,38 +6042,40 @@
       <c r="BZ33" s="11"/>
       <c r="CA33" s="11"/>
     </row>
-    <row r="34" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B34" s="5">
         <v>29</v>
       </c>
-      <c r="C34" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="17">
-        <v>3</v>
-      </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18">
+      <c r="C34" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="16">
+        <v>4</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17">
         <v>1</v>
       </c>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18">
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17">
         <v>1</v>
       </c>
-      <c r="T34" s="18"/>
-      <c r="U34" s="11"/>
-      <c r="V34" s="11"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17">
+        <v>1</v>
+      </c>
       <c r="W34" s="11"/>
       <c r="X34" s="11"/>
       <c r="Y34" s="11"/>
@@ -6112,12 +6134,12 @@
       <c r="BZ34" s="11"/>
       <c r="CA34" s="11"/>
     </row>
-    <row r="35" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B35" s="5">
         <v>30</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>111</v>
+      <c r="C35" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="D35" s="12">
         <v>4</v>
@@ -6198,12 +6220,12 @@
       <c r="BZ35" s="11"/>
       <c r="CA35" s="11"/>
     </row>
-    <row r="36" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B36" s="5">
         <v>31</v>
       </c>
-      <c r="C36" s="19" t="s">
-        <v>112</v>
+      <c r="C36" s="18" t="s">
+        <v>111</v>
       </c>
       <c r="D36" s="12">
         <v>2</v>
@@ -6284,15 +6306,15 @@
       <c r="BZ36" s="11"/>
       <c r="CA36" s="11"/>
     </row>
-    <row r="37" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B37" s="5">
         <v>32</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>113</v>
+      <c r="C37" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="D37" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -6370,15 +6392,15 @@
       <c r="BZ37" s="11"/>
       <c r="CA37" s="11"/>
     </row>
-    <row r="38" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B38" s="5">
         <v>33</v>
       </c>
-      <c r="C38" s="19" t="s">
-        <v>114</v>
+      <c r="C38" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="D38" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -6456,11 +6478,13 @@
       <c r="BZ38" s="11"/>
       <c r="CA38" s="11"/>
     </row>
-    <row r="39" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B39" s="5">
         <v>34</v>
       </c>
-      <c r="C39" s="11"/>
+      <c r="C39" s="24" t="s">
+        <v>115</v>
+      </c>
       <c r="D39" s="12">
         <v>1</v>
       </c>
@@ -6540,11 +6564,13 @@
       <c r="BZ39" s="11"/>
       <c r="CA39" s="11"/>
     </row>
-    <row r="40" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B40" s="5">
         <v>35</v>
       </c>
-      <c r="C40" s="11"/>
+      <c r="C40" s="24" t="s">
+        <v>118</v>
+      </c>
       <c r="D40" s="12">
         <v>1</v>
       </c>
@@ -6624,12 +6650,16 @@
       <c r="BZ40" s="11"/>
       <c r="CA40" s="11"/>
     </row>
-    <row r="41" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B41" s="5">
         <v>36</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12"/>
+      <c r="C41" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="12">
+        <v>1</v>
+      </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -6706,12 +6736,16 @@
       <c r="BZ41" s="11"/>
       <c r="CA41" s="11"/>
     </row>
-    <row r="42" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B42" s="5">
         <v>37</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12"/>
+      <c r="C42" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="12">
+        <v>1</v>
+      </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -6788,7 +6822,7 @@
       <c r="BZ42" s="11"/>
       <c r="CA42" s="11"/>
     </row>
-    <row r="43" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B43" s="5">
         <v>38</v>
       </c>
@@ -6870,7 +6904,7 @@
       <c r="BZ43" s="11"/>
       <c r="CA43" s="11"/>
     </row>
-    <row r="44" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B44" s="5">
         <v>39</v>
       </c>
@@ -6952,7 +6986,7 @@
       <c r="BZ44" s="11"/>
       <c r="CA44" s="11"/>
     </row>
-    <row r="45" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B45" s="5">
         <v>40</v>
       </c>
@@ -7034,7 +7068,7 @@
       <c r="BZ45" s="11"/>
       <c r="CA45" s="11"/>
     </row>
-    <row r="46" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B46" s="5">
         <v>41</v>
       </c>
@@ -7116,7 +7150,7 @@
       <c r="BZ46" s="11"/>
       <c r="CA46" s="11"/>
     </row>
-    <row r="47" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B47" s="5">
         <v>42</v>
       </c>
@@ -7198,7 +7232,7 @@
       <c r="BZ47" s="11"/>
       <c r="CA47" s="11"/>
     </row>
-    <row r="48" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B48" s="5">
         <v>43</v>
       </c>
@@ -7280,7 +7314,7 @@
       <c r="BZ48" s="11"/>
       <c r="CA48" s="11"/>
     </row>
-    <row r="49" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B49" s="5">
         <v>44</v>
       </c>
@@ -7362,7 +7396,7 @@
       <c r="BZ49" s="11"/>
       <c r="CA49" s="11"/>
     </row>
-    <row r="50" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B50" s="5">
         <v>45</v>
       </c>
@@ -7444,7 +7478,7 @@
       <c r="BZ50" s="11"/>
       <c r="CA50" s="11"/>
     </row>
-    <row r="51" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B51" s="5">
         <v>46</v>
       </c>
@@ -7526,7 +7560,7 @@
       <c r="BZ51" s="11"/>
       <c r="CA51" s="11"/>
     </row>
-    <row r="52" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B52" s="5">
         <v>47</v>
       </c>
@@ -7608,7 +7642,7 @@
       <c r="BZ52" s="11"/>
       <c r="CA52" s="11"/>
     </row>
-    <row r="53" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B53" s="5">
         <v>48</v>
       </c>
@@ -7690,7 +7724,7 @@
       <c r="BZ53" s="11"/>
       <c r="CA53" s="11"/>
     </row>
-    <row r="54" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B54" s="5">
         <v>49</v>
       </c>
@@ -7772,7 +7806,7 @@
       <c r="BZ54" s="11"/>
       <c r="CA54" s="11"/>
     </row>
-    <row r="55" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B55" s="5">
         <v>50</v>
       </c>
@@ -7854,7 +7888,7 @@
       <c r="BZ55" s="11"/>
       <c r="CA55" s="11"/>
     </row>
-    <row r="56" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B56" s="5">
         <v>51</v>
       </c>
@@ -7936,7 +7970,7 @@
       <c r="BZ56" s="11"/>
       <c r="CA56" s="11"/>
     </row>
-    <row r="57" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B57" s="5">
         <v>52</v>
       </c>
@@ -8018,7 +8052,7 @@
       <c r="BZ57" s="11"/>
       <c r="CA57" s="11"/>
     </row>
-    <row r="58" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B58" s="5">
         <v>53</v>
       </c>
@@ -8100,7 +8134,7 @@
       <c r="BZ58" s="11"/>
       <c r="CA58" s="11"/>
     </row>
-    <row r="59" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B59" s="5">
         <v>54</v>
       </c>
@@ -8182,7 +8216,7 @@
       <c r="BZ59" s="11"/>
       <c r="CA59" s="11"/>
     </row>
-    <row r="60" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B60" s="5">
         <v>55</v>
       </c>
@@ -8264,7 +8298,7 @@
       <c r="BZ60" s="11"/>
       <c r="CA60" s="11"/>
     </row>
-    <row r="61" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B61" s="5">
         <v>56</v>
       </c>
@@ -8346,7 +8380,7 @@
       <c r="BZ61" s="11"/>
       <c r="CA61" s="11"/>
     </row>
-    <row r="62" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B62" s="5">
         <v>57</v>
       </c>
@@ -8428,7 +8462,7 @@
       <c r="BZ62" s="11"/>
       <c r="CA62" s="11"/>
     </row>
-    <row r="63" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B63" s="5">
         <v>58</v>
       </c>
@@ -8510,7 +8544,7 @@
       <c r="BZ63" s="11"/>
       <c r="CA63" s="11"/>
     </row>
-    <row r="64" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B64" s="5">
         <v>59</v>
       </c>
@@ -8592,7 +8626,7 @@
       <c r="BZ64" s="11"/>
       <c r="CA64" s="11"/>
     </row>
-    <row r="65" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B65" s="5">
         <v>60</v>
       </c>
@@ -8674,7 +8708,7 @@
       <c r="BZ65" s="11"/>
       <c r="CA65" s="11"/>
     </row>
-    <row r="66" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B66" s="5">
         <v>61</v>
       </c>
@@ -8756,7 +8790,7 @@
       <c r="BZ66" s="11"/>
       <c r="CA66" s="11"/>
     </row>
-    <row r="67" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B67" s="5">
         <v>62</v>
       </c>
@@ -8838,7 +8872,7 @@
       <c r="BZ67" s="11"/>
       <c r="CA67" s="11"/>
     </row>
-    <row r="68" spans="2:79" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:79" x14ac:dyDescent="0.3">
       <c r="B68" s="5">
         <v>63</v>
       </c>
@@ -8920,11 +8954,11 @@
       <c r="BZ68" s="11"/>
       <c r="CA68" s="11"/>
     </row>
-    <row r="69" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B69" s="22" t="s">
+    <row r="69" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B69" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="22"/>
+      <c r="C69" s="21"/>
       <c r="D69" s="6">
         <f>SUM(D6:D68)</f>
         <v>63</v>
@@ -8999,242 +9033,242 @@
       </c>
       <c r="V69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="W69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="X69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Y69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="70" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B70" s="21" t="s">
+    <row r="70" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B70" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="21"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="3">
         <f>SUM(D6:D68)</f>
         <v>63</v>

</xml_diff>

<commit_message>
Account form for update, delete.
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD343DA1-F24D-4CE7-8E5E-7CF6993764E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDCCA7D-727A-40E4-80A6-F622FEA143A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -372,9 +372,6 @@
   </si>
   <si>
     <t>Data Bewaar Limiet</t>
-  </si>
-  <si>
-    <t>Foto Uploaden</t>
   </si>
   <si>
     <t>Zoekfilters</t>
@@ -474,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,12 +499,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -594,13 +585,13 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -624,8 +615,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1050,187 +1041,187 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2915,8 +2906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3562,7 +3553,7 @@
       <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>79</v>
       </c>
       <c r="D6" s="13">
@@ -3652,7 +3643,7 @@
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>82</v>
       </c>
       <c r="D7" s="13">
@@ -3830,7 +3821,7 @@
       <c r="B9" s="5">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>101</v>
       </c>
       <c r="D9" s="13">
@@ -3918,7 +3909,7 @@
       <c r="B10" s="5">
         <v>5</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>102</v>
       </c>
       <c r="D10" s="13">
@@ -4006,7 +3997,7 @@
       <c r="B11" s="5">
         <v>6</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D11" s="13">
@@ -4094,7 +4085,7 @@
       <c r="B12" s="5">
         <v>7</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>81</v>
       </c>
       <c r="D12" s="13">
@@ -4190,7 +4181,7 @@
       <c r="B13" s="5">
         <v>8</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>83</v>
       </c>
       <c r="D13" s="13">
@@ -4278,7 +4269,7 @@
       <c r="B14" s="5">
         <v>9</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>84</v>
       </c>
       <c r="D14" s="13">
@@ -4366,7 +4357,7 @@
       <c r="B15" s="5">
         <v>10</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="13">
@@ -4454,7 +4445,7 @@
       <c r="B16" s="5">
         <v>11</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>86</v>
       </c>
       <c r="D16" s="13">
@@ -4542,10 +4533,10 @@
       <c r="B17" s="5">
         <v>12</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="15">
         <v>2</v>
       </c>
       <c r="E17" s="11"/>
@@ -4566,7 +4557,9 @@
       <c r="T17" s="11"/>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
+      <c r="W17" s="16">
+        <v>1</v>
+      </c>
       <c r="X17" s="11"/>
       <c r="Y17" s="11"/>
       <c r="Z17" s="11"/>
@@ -4628,10 +4621,10 @@
       <c r="B18" s="5">
         <v>13</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="15">
         <v>2</v>
       </c>
       <c r="E18" s="11"/>
@@ -4652,7 +4645,9 @@
       <c r="T18" s="11"/>
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
+      <c r="W18" s="16">
+        <v>1</v>
+      </c>
       <c r="X18" s="11"/>
       <c r="Y18" s="11"/>
       <c r="Z18" s="11"/>
@@ -4714,7 +4709,7 @@
       <c r="B19" s="5">
         <v>14</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>89</v>
       </c>
       <c r="D19" s="13">
@@ -4802,7 +4797,7 @@
       <c r="B20" s="5">
         <v>15</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D20" s="13">
@@ -4890,7 +4885,7 @@
       <c r="B21" s="5">
         <v>16</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>90</v>
       </c>
       <c r="D21" s="13">
@@ -4913,7 +4908,7 @@
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
-      <c r="T21" s="17">
+      <c r="T21" s="16">
         <v>-1</v>
       </c>
       <c r="U21" s="1">
@@ -4982,7 +4977,7 @@
       <c r="B22" s="5">
         <v>17</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>91</v>
       </c>
       <c r="D22" s="13">
@@ -5070,7 +5065,7 @@
       <c r="B23" s="5">
         <v>18</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>92</v>
       </c>
       <c r="D23" s="13">
@@ -5093,7 +5088,7 @@
       </c>
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
-      <c r="T23" s="17">
+      <c r="T23" s="16">
         <v>-1</v>
       </c>
       <c r="U23" s="1">
@@ -5162,7 +5157,7 @@
       <c r="B24" s="5">
         <v>19</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>93</v>
       </c>
       <c r="D24" s="13">
@@ -5250,7 +5245,7 @@
       <c r="B25" s="5">
         <v>20</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>94</v>
       </c>
       <c r="D25" s="13">
@@ -5338,7 +5333,7 @@
       <c r="B26" s="5">
         <v>21</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>96</v>
       </c>
       <c r="D26" s="13">
@@ -5518,7 +5513,7 @@
       <c r="B28" s="5">
         <v>23</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="14" t="s">
         <v>103</v>
       </c>
       <c r="D28" s="13">
@@ -5606,7 +5601,7 @@
       <c r="B29" s="5">
         <v>24</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="14" t="s">
         <v>104</v>
       </c>
       <c r="D29" s="13">
@@ -5694,7 +5689,7 @@
       <c r="B30" s="5">
         <v>25</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>106</v>
       </c>
       <c r="D30" s="13">
@@ -5782,7 +5777,7 @@
       <c r="B31" s="5">
         <v>26</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="14" t="s">
         <v>107</v>
       </c>
       <c r="D31" s="13">
@@ -5870,7 +5865,7 @@
       <c r="B32" s="5">
         <v>27</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="14" t="s">
         <v>108</v>
       </c>
       <c r="D32" s="13">
@@ -5959,7 +5954,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D33" s="13">
         <v>1</v>
@@ -6046,34 +6041,34 @@
       <c r="B34" s="5">
         <v>29</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="16">
+      <c r="D34" s="15">
         <v>4</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17">
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16">
         <v>1</v>
       </c>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
-      <c r="S34" s="17">
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16">
         <v>1</v>
       </c>
-      <c r="T34" s="17"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17">
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16">
         <v>1</v>
       </c>
       <c r="W34" s="11"/>
@@ -6138,7 +6133,7 @@
       <c r="B35" s="5">
         <v>30</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="17" t="s">
         <v>110</v>
       </c>
       <c r="D35" s="12">
@@ -6224,7 +6219,7 @@
       <c r="B36" s="5">
         <v>31</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="17" t="s">
         <v>111</v>
       </c>
       <c r="D36" s="12">
@@ -6310,8 +6305,8 @@
       <c r="B37" s="5">
         <v>32</v>
       </c>
-      <c r="C37" s="18" t="s">
-        <v>112</v>
+      <c r="C37" s="17" t="s">
+        <v>116</v>
       </c>
       <c r="D37" s="12">
         <v>1</v>
@@ -6396,11 +6391,11 @@
       <c r="B38" s="5">
         <v>33</v>
       </c>
-      <c r="C38" s="18" t="s">
-        <v>113</v>
+      <c r="C38" s="17" t="s">
+        <v>112</v>
       </c>
       <c r="D38" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -6482,10 +6477,10 @@
       <c r="B39" s="5">
         <v>34</v>
       </c>
-      <c r="C39" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="12">
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="13">
         <v>1</v>
       </c>
       <c r="E39" s="11"/>
@@ -6502,11 +6497,17 @@
       <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="11"/>
-      <c r="V39" s="11"/>
-      <c r="W39" s="11"/>
+      <c r="S39" s="1">
+        <v>1</v>
+      </c>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="16">
+        <v>-1</v>
+      </c>
+      <c r="W39" s="1">
+        <v>1</v>
+      </c>
       <c r="X39" s="11"/>
       <c r="Y39" s="11"/>
       <c r="Z39" s="11"/>
@@ -6568,8 +6569,8 @@
       <c r="B40" s="5">
         <v>35</v>
       </c>
-      <c r="C40" s="24" t="s">
-        <v>118</v>
+      <c r="C40" s="18" t="s">
+        <v>117</v>
       </c>
       <c r="D40" s="12">
         <v>1</v>
@@ -6654,8 +6655,8 @@
       <c r="B41" s="5">
         <v>36</v>
       </c>
-      <c r="C41" s="24" t="s">
-        <v>116</v>
+      <c r="C41" s="18" t="s">
+        <v>115</v>
       </c>
       <c r="D41" s="12">
         <v>1</v>
@@ -6740,12 +6741,8 @@
       <c r="B42" s="5">
         <v>37</v>
       </c>
-      <c r="C42" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="12">
-        <v>1</v>
-      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -9021,15 +9018,15 @@
       </c>
       <c r="S69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="T69" s="7">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U69" s="7">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V69" s="7">
         <f t="shared" si="1"/>
@@ -9037,231 +9034,231 @@
       </c>
       <c r="W69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="X69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Y69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Zoek velden, admin panel, docs update
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDCCA7D-727A-40E4-80A6-F622FEA143A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140C212C-5564-43E7-980B-59E2D840F062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -600,6 +600,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -614,9 +617,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1032,196 +1032,196 @@
                   <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33</c:v>
+                  <c:v>33.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>15</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2906,8 +2906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2920,172 +2920,172 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:79" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="19"/>
-      <c r="AQ2" s="19"/>
-      <c r="AR2" s="19"/>
-      <c r="AS2" s="19"/>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="19"/>
-      <c r="BH2" s="19"/>
-      <c r="BI2" s="19"/>
-      <c r="BJ2" s="19"/>
-      <c r="BK2" s="19"/>
-      <c r="BL2" s="19"/>
-      <c r="BM2" s="19"/>
-      <c r="BN2" s="19"/>
-      <c r="BO2" s="19"/>
-      <c r="BP2" s="19"/>
-      <c r="BQ2" s="19"/>
-      <c r="BR2" s="19"/>
-      <c r="BS2" s="19"/>
-      <c r="BT2" s="19"/>
-      <c r="BU2" s="19"/>
-      <c r="BV2" s="19"/>
-      <c r="BW2" s="19"/>
-      <c r="BX2" s="19"/>
-      <c r="BY2" s="19"/>
-      <c r="BZ2" s="19"/>
-      <c r="CA2" s="19"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="20"/>
+      <c r="BD2" s="20"/>
+      <c r="BE2" s="20"/>
+      <c r="BF2" s="20"/>
+      <c r="BG2" s="20"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
+      <c r="BK2" s="20"/>
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="20"/>
+      <c r="BN2" s="20"/>
+      <c r="BO2" s="20"/>
+      <c r="BP2" s="20"/>
+      <c r="BQ2" s="20"/>
+      <c r="BR2" s="20"/>
+      <c r="BS2" s="20"/>
+      <c r="BT2" s="20"/>
+      <c r="BU2" s="20"/>
+      <c r="BV2" s="20"/>
+      <c r="BW2" s="20"/>
+      <c r="BX2" s="20"/>
+      <c r="BY2" s="20"/>
+      <c r="BZ2" s="20"/>
+      <c r="CA2" s="20"/>
     </row>
     <row r="3" spans="2:79" x14ac:dyDescent="0.3">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="19"/>
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19"/>
-      <c r="AL3" s="19"/>
-      <c r="AM3" s="19"/>
-      <c r="AN3" s="19"/>
-      <c r="AO3" s="19"/>
-      <c r="AP3" s="19"/>
-      <c r="AQ3" s="19"/>
-      <c r="AR3" s="19"/>
-      <c r="AS3" s="19"/>
-      <c r="AT3" s="19"/>
-      <c r="AU3" s="19"/>
-      <c r="AV3" s="19"/>
-      <c r="AW3" s="19"/>
-      <c r="AX3" s="19"/>
-      <c r="AY3" s="19"/>
-      <c r="AZ3" s="19"/>
-      <c r="BA3" s="19"/>
-      <c r="BB3" s="19"/>
-      <c r="BC3" s="19"/>
-      <c r="BD3" s="19"/>
-      <c r="BE3" s="19"/>
-      <c r="BF3" s="19"/>
-      <c r="BG3" s="19"/>
-      <c r="BH3" s="19"/>
-      <c r="BI3" s="19"/>
-      <c r="BJ3" s="19"/>
-      <c r="BK3" s="19"/>
-      <c r="BL3" s="19"/>
-      <c r="BM3" s="19"/>
-      <c r="BN3" s="19"/>
-      <c r="BO3" s="19"/>
-      <c r="BP3" s="19"/>
-      <c r="BQ3" s="19"/>
-      <c r="BR3" s="19"/>
-      <c r="BS3" s="19"/>
-      <c r="BT3" s="19"/>
-      <c r="BU3" s="19"/>
-      <c r="BV3" s="19"/>
-      <c r="BW3" s="19"/>
-      <c r="BX3" s="19"/>
-      <c r="BY3" s="19"/>
-      <c r="BZ3" s="19"/>
-      <c r="CA3" s="19"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20"/>
+      <c r="AH3" s="20"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="20"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+      <c r="BB3" s="20"/>
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="20"/>
+      <c r="BE3" s="20"/>
+      <c r="BF3" s="20"/>
+      <c r="BG3" s="20"/>
+      <c r="BH3" s="20"/>
+      <c r="BI3" s="20"/>
+      <c r="BJ3" s="20"/>
+      <c r="BK3" s="20"/>
+      <c r="BL3" s="20"/>
+      <c r="BM3" s="20"/>
+      <c r="BN3" s="20"/>
+      <c r="BO3" s="20"/>
+      <c r="BP3" s="20"/>
+      <c r="BQ3" s="20"/>
+      <c r="BR3" s="20"/>
+      <c r="BS3" s="20"/>
+      <c r="BT3" s="20"/>
+      <c r="BU3" s="20"/>
+      <c r="BV3" s="20"/>
+      <c r="BW3" s="20"/>
+      <c r="BX3" s="20"/>
+      <c r="BY3" s="20"/>
+      <c r="BZ3" s="20"/>
+      <c r="CA3" s="20"/>
     </row>
     <row r="4" spans="2:79" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -3318,8 +3318,8 @@
       </c>
     </row>
     <row r="5" spans="2:79" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
@@ -3663,15 +3663,17 @@
         <v>0.5</v>
       </c>
       <c r="P7" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1">
+        <v>0.5</v>
+      </c>
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
       <c r="Z7" s="11"/>
@@ -4533,7 +4535,7 @@
       <c r="B17" s="5">
         <v>12</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="19" t="s">
         <v>87</v>
       </c>
       <c r="D17" s="15">
@@ -4621,7 +4623,7 @@
       <c r="B18" s="5">
         <v>13</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="19" t="s">
         <v>88</v>
       </c>
       <c r="D18" s="15">
@@ -6069,7 +6071,7 @@
       <c r="T34" s="16"/>
       <c r="U34" s="16"/>
       <c r="V34" s="16">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="W34" s="11"/>
       <c r="X34" s="11"/>
@@ -6391,10 +6393,10 @@
       <c r="B38" s="5">
         <v>33</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="15">
         <v>3</v>
       </c>
       <c r="E38" s="11"/>
@@ -6414,7 +6416,9 @@
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
       <c r="U38" s="11"/>
-      <c r="V38" s="11"/>
+      <c r="V38" s="16">
+        <v>2</v>
+      </c>
       <c r="W38" s="11"/>
       <c r="X38" s="11"/>
       <c r="Y38" s="11"/>
@@ -8952,10 +8956,10 @@
       <c r="CA68" s="11"/>
     </row>
     <row r="69" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="21"/>
+      <c r="C69" s="22"/>
       <c r="D69" s="6">
         <f>SUM(D6:D68)</f>
         <v>63</v>
@@ -9006,266 +9010,266 @@
       </c>
       <c r="P69" s="7">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>33.5</v>
       </c>
       <c r="Q69" s="7">
         <f t="shared" ref="Q69:AV69" si="1">P69-SUM(Q6:Q68)</f>
-        <v>21</v>
+        <v>21.5</v>
       </c>
       <c r="R69" s="7">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>21.5</v>
       </c>
       <c r="S69" s="7">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="T69" s="7">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>22.5</v>
       </c>
       <c r="U69" s="7">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="V69" s="7">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="W69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="X69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="Y69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="70" spans="2:79" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="20"/>
+      <c r="C70" s="21"/>
       <c r="D70" s="3">
         <f>SUM(D6:D68)</f>
         <v>63</v>

</xml_diff>

<commit_message>
Nieuwe Definition of Done & Fun
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF05B98A-C1C0-408E-9AA9-00C7F7D683D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C70C873-7FC6-489B-8DE3-FBDB30EAB3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -390,6 +390,12 @@
   </si>
   <si>
     <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Definition of Done</t>
+  </si>
+  <si>
+    <t>Definition of Fun</t>
   </si>
 </sst>
 </file>
@@ -1062,166 +1068,166 @@
                   <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>11.5</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2906,8 +2912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="O33" workbookViewId="0">
+      <selection activeCell="Z47" sqref="Z47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4562,9 +4568,9 @@
       <c r="W17" s="16">
         <v>1</v>
       </c>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="16"/>
       <c r="AA17" s="11"/>
       <c r="AB17" s="11"/>
       <c r="AC17" s="11"/>
@@ -4650,9 +4656,9 @@
       <c r="W18" s="16">
         <v>1</v>
       </c>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="16"/>
       <c r="AA18" s="11"/>
       <c r="AB18" s="11"/>
       <c r="AC18" s="11"/>
@@ -6139,7 +6145,7 @@
         <v>110</v>
       </c>
       <c r="D35" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -6747,8 +6753,12 @@
       <c r="B42" s="5">
         <v>37</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12"/>
+      <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="13">
+        <v>1</v>
+      </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
@@ -6770,7 +6780,9 @@
       <c r="W42" s="11"/>
       <c r="X42" s="11"/>
       <c r="Y42" s="11"/>
-      <c r="Z42" s="11"/>
+      <c r="Z42" s="1">
+        <v>1</v>
+      </c>
       <c r="AA42" s="11"/>
       <c r="AB42" s="11"/>
       <c r="AC42" s="11"/>
@@ -6829,8 +6841,12 @@
       <c r="B43" s="5">
         <v>38</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="12"/>
+      <c r="C43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="13">
+        <v>1</v>
+      </c>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -6852,7 +6868,9 @@
       <c r="W43" s="11"/>
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
-      <c r="Z43" s="11"/>
+      <c r="Z43" s="1">
+        <v>1</v>
+      </c>
       <c r="AA43" s="11"/>
       <c r="AB43" s="11"/>
       <c r="AC43" s="11"/>
@@ -9052,219 +9070,219 @@
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="70" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Major update, css, forms, server message. Added date calculators
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0413FAB-8512-4D5A-B425-8AD5CDEB7CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBEE33B-7EF5-45CC-8620-78D4D05E4BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -287,9 +287,6 @@
     <t>Resp. Design &amp; CSS</t>
   </si>
   <si>
-    <t>Navigatie Bar</t>
-  </si>
-  <si>
     <t>Gemeentelijk Logo</t>
   </si>
   <si>
@@ -353,15 +350,9 @@
     <t>Makkelijk Ontwerp</t>
   </si>
   <si>
-    <t>Gebruikersnaam</t>
-  </si>
-  <si>
     <t>Inlog Formulier</t>
   </si>
   <si>
-    <t>Registreer Formulier</t>
-  </si>
-  <si>
     <t>Klachten Formulier</t>
   </si>
   <si>
@@ -377,9 +368,6 @@
     <t>Zoekfilters</t>
   </si>
   <si>
-    <t>Gegevens sturen PHP</t>
-  </si>
-  <si>
     <t>Use Case Diagram</t>
   </si>
   <si>
@@ -396,6 +384,24 @@
   </si>
   <si>
     <t>Definition of Fun</t>
+  </si>
+  <si>
+    <t>Display Gebruiker</t>
+  </si>
+  <si>
+    <t>Navigatie Balk</t>
+  </si>
+  <si>
+    <t>Registratie Formulier</t>
+  </si>
+  <si>
+    <t>Afgerond</t>
+  </si>
+  <si>
+    <t>Bezig…</t>
+  </si>
+  <si>
+    <t>Veiligheidstaken</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFCCFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,9 +600,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -615,6 +618,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -624,6 +633,7 @@
   <colors>
     <mruColors>
       <color rgb="FF99FF99"/>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FF9999FF"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FF66FF66"/>
@@ -708,7 +718,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1017,88 +1027,88 @@
                   <c:v>56.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.5</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>33.5</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>22.5</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>22.5</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>23.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20.5</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>17</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="22">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="31">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.5</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8.5</c:v>
-                </c:pt>
                 <c:pt idx="32">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>7</c:v>
@@ -1107,118 +1117,118 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1813,7 +1823,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1750577888"/>
@@ -1882,7 +1892,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1495853808"/>
@@ -1923,7 +1933,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1963,7 +1973,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2903,8 +2913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="AO39" sqref="AO39"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2917,176 +2927,176 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:79" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="19"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-      <c r="AH2" s="19"/>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="19"/>
-      <c r="AP2" s="19"/>
-      <c r="AQ2" s="19"/>
-      <c r="AR2" s="19"/>
-      <c r="AS2" s="19"/>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="19"/>
-      <c r="AX2" s="19"/>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="19"/>
-      <c r="BF2" s="19"/>
-      <c r="BG2" s="19"/>
-      <c r="BH2" s="19"/>
-      <c r="BI2" s="19"/>
-      <c r="BJ2" s="19"/>
-      <c r="BK2" s="19"/>
-      <c r="BL2" s="19"/>
-      <c r="BM2" s="19"/>
-      <c r="BN2" s="19"/>
-      <c r="BO2" s="19"/>
-      <c r="BP2" s="19"/>
-      <c r="BQ2" s="19"/>
-      <c r="BR2" s="19"/>
-      <c r="BS2" s="19"/>
-      <c r="BT2" s="19"/>
-      <c r="BU2" s="19"/>
-      <c r="BV2" s="19"/>
-      <c r="BW2" s="19"/>
-      <c r="BX2" s="19"/>
-      <c r="BY2" s="19"/>
-      <c r="BZ2" s="19"/>
-      <c r="CA2" s="19"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
+      <c r="AR2" s="18"/>
+      <c r="AS2" s="18"/>
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="18"/>
+      <c r="AV2" s="18"/>
+      <c r="AW2" s="18"/>
+      <c r="AX2" s="18"/>
+      <c r="AY2" s="18"/>
+      <c r="AZ2" s="18"/>
+      <c r="BA2" s="18"/>
+      <c r="BB2" s="18"/>
+      <c r="BC2" s="18"/>
+      <c r="BD2" s="18"/>
+      <c r="BE2" s="18"/>
+      <c r="BF2" s="18"/>
+      <c r="BG2" s="18"/>
+      <c r="BH2" s="18"/>
+      <c r="BI2" s="18"/>
+      <c r="BJ2" s="18"/>
+      <c r="BK2" s="18"/>
+      <c r="BL2" s="18"/>
+      <c r="BM2" s="18"/>
+      <c r="BN2" s="18"/>
+      <c r="BO2" s="18"/>
+      <c r="BP2" s="18"/>
+      <c r="BQ2" s="18"/>
+      <c r="BR2" s="18"/>
+      <c r="BS2" s="18"/>
+      <c r="BT2" s="18"/>
+      <c r="BU2" s="18"/>
+      <c r="BV2" s="18"/>
+      <c r="BW2" s="18"/>
+      <c r="BX2" s="18"/>
+      <c r="BY2" s="18"/>
+      <c r="BZ2" s="18"/>
+      <c r="CA2" s="18"/>
     </row>
     <row r="3" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="19"/>
-      <c r="AJ3" s="19"/>
-      <c r="AK3" s="19"/>
-      <c r="AL3" s="19"/>
-      <c r="AM3" s="19"/>
-      <c r="AN3" s="19"/>
-      <c r="AO3" s="19"/>
-      <c r="AP3" s="19"/>
-      <c r="AQ3" s="19"/>
-      <c r="AR3" s="19"/>
-      <c r="AS3" s="19"/>
-      <c r="AT3" s="19"/>
-      <c r="AU3" s="19"/>
-      <c r="AV3" s="19"/>
-      <c r="AW3" s="19"/>
-      <c r="AX3" s="19"/>
-      <c r="AY3" s="19"/>
-      <c r="AZ3" s="19"/>
-      <c r="BA3" s="19"/>
-      <c r="BB3" s="19"/>
-      <c r="BC3" s="19"/>
-      <c r="BD3" s="19"/>
-      <c r="BE3" s="19"/>
-      <c r="BF3" s="19"/>
-      <c r="BG3" s="19"/>
-      <c r="BH3" s="19"/>
-      <c r="BI3" s="19"/>
-      <c r="BJ3" s="19"/>
-      <c r="BK3" s="19"/>
-      <c r="BL3" s="19"/>
-      <c r="BM3" s="19"/>
-      <c r="BN3" s="19"/>
-      <c r="BO3" s="19"/>
-      <c r="BP3" s="19"/>
-      <c r="BQ3" s="19"/>
-      <c r="BR3" s="19"/>
-      <c r="BS3" s="19"/>
-      <c r="BT3" s="19"/>
-      <c r="BU3" s="19"/>
-      <c r="BV3" s="19"/>
-      <c r="BW3" s="19"/>
-      <c r="BX3" s="19"/>
-      <c r="BY3" s="19"/>
-      <c r="BZ3" s="19"/>
-      <c r="CA3" s="19"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="18"/>
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="18"/>
+      <c r="AH3" s="18"/>
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="18"/>
+      <c r="AM3" s="18"/>
+      <c r="AN3" s="18"/>
+      <c r="AO3" s="18"/>
+      <c r="AP3" s="18"/>
+      <c r="AQ3" s="18"/>
+      <c r="AR3" s="18"/>
+      <c r="AS3" s="18"/>
+      <c r="AT3" s="18"/>
+      <c r="AU3" s="18"/>
+      <c r="AV3" s="18"/>
+      <c r="AW3" s="18"/>
+      <c r="AX3" s="18"/>
+      <c r="AY3" s="18"/>
+      <c r="AZ3" s="18"/>
+      <c r="BA3" s="18"/>
+      <c r="BB3" s="18"/>
+      <c r="BC3" s="18"/>
+      <c r="BD3" s="18"/>
+      <c r="BE3" s="18"/>
+      <c r="BF3" s="18"/>
+      <c r="BG3" s="18"/>
+      <c r="BH3" s="18"/>
+      <c r="BI3" s="18"/>
+      <c r="BJ3" s="18"/>
+      <c r="BK3" s="18"/>
+      <c r="BL3" s="18"/>
+      <c r="BM3" s="18"/>
+      <c r="BN3" s="18"/>
+      <c r="BO3" s="18"/>
+      <c r="BP3" s="18"/>
+      <c r="BQ3" s="18"/>
+      <c r="BR3" s="18"/>
+      <c r="BS3" s="18"/>
+      <c r="BT3" s="18"/>
+      <c r="BU3" s="18"/>
+      <c r="BV3" s="18"/>
+      <c r="BW3" s="18"/>
+      <c r="BX3" s="18"/>
+      <c r="BY3" s="18"/>
+      <c r="BZ3" s="18"/>
+      <c r="CA3" s="18"/>
     </row>
     <row r="4" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="9">
         <v>45243</v>
@@ -3315,8 +3325,8 @@
       </c>
     </row>
     <row r="5" spans="2:79" x14ac:dyDescent="0.35">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
@@ -3821,7 +3831,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="13">
         <v>1</v>
@@ -3909,7 +3919,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="13">
         <v>0.5</v>
@@ -3997,7 +4007,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D11" s="13">
         <v>0.5</v>
@@ -4181,7 +4191,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="D13" s="13">
         <v>2</v>
@@ -4269,10 +4279,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4285,7 +4295,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
@@ -4357,7 +4367,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" s="13">
         <v>2</v>
@@ -4445,7 +4455,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="13">
         <v>2</v>
@@ -4532,10 +4542,10 @@
       <c r="B17" s="5">
         <v>12</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="15">
+      <c r="C17" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="13">
         <v>2</v>
       </c>
       <c r="E17" s="11"/>
@@ -4574,8 +4584,10 @@
       <c r="AJ17" s="16"/>
       <c r="AK17" s="16"/>
       <c r="AL17" s="16"/>
-      <c r="AM17" s="16"/>
-      <c r="AN17" s="16"/>
+      <c r="AM17" s="11"/>
+      <c r="AN17" s="1">
+        <v>1</v>
+      </c>
       <c r="AO17" s="11"/>
       <c r="AP17" s="11"/>
       <c r="AQ17" s="11"/>
@@ -4620,8 +4632,8 @@
       <c r="B18" s="5">
         <v>13</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>88</v>
+      <c r="C18" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="D18" s="15">
         <v>2</v>
@@ -4664,8 +4676,8 @@
       <c r="AL18" s="16"/>
       <c r="AM18" s="16"/>
       <c r="AN18" s="16"/>
-      <c r="AO18" s="11"/>
-      <c r="AP18" s="11"/>
+      <c r="AO18" s="16"/>
+      <c r="AP18" s="16"/>
       <c r="AQ18" s="11"/>
       <c r="AR18" s="11"/>
       <c r="AS18" s="11"/>
@@ -4709,7 +4721,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D19" s="13">
         <v>2</v>
@@ -4796,11 +4808,11 @@
       <c r="B20" s="5">
         <v>15</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>95</v>
+      <c r="C20" s="24" t="s">
+        <v>94</v>
       </c>
       <c r="D20" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -4810,7 +4822,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
@@ -4885,7 +4897,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="13">
         <v>2</v>
@@ -4977,7 +4989,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="13">
         <v>2</v>
@@ -5065,7 +5077,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -5157,7 +5169,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="13">
         <v>2</v>
@@ -5245,7 +5257,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25" s="13">
         <v>2</v>
@@ -5335,7 +5347,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D26" s="13">
         <v>1</v>
@@ -5427,7 +5439,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D27" s="13">
         <v>1</v>
@@ -5515,7 +5527,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="13">
         <v>1</v>
@@ -5603,7 +5615,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D29" s="13">
         <v>1</v>
@@ -5691,7 +5703,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D30" s="13">
         <v>1</v>
@@ -5779,7 +5791,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D31" s="13">
         <v>1</v>
@@ -5867,7 +5879,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D32" s="13">
         <v>1</v>
@@ -5954,11 +5966,11 @@
       <c r="B33" s="5">
         <v>28</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>113</v>
+      <c r="C33" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="D33" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -5967,33 +5979,41 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="1">
+      <c r="L33" s="16">
         <v>1</v>
       </c>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
-      <c r="AE33" s="11"/>
-      <c r="AF33" s="11"/>
-      <c r="AG33" s="11"/>
-      <c r="AH33" s="11"/>
-      <c r="AI33" s="11"/>
-      <c r="AJ33" s="11"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="16">
+        <v>1</v>
+      </c>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="16">
+        <v>1</v>
+      </c>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1"/>
+      <c r="AH33" s="1"/>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="1">
+        <v>1</v>
+      </c>
       <c r="AK33" s="11"/>
       <c r="AL33" s="11"/>
       <c r="AM33" s="11"/>
@@ -6042,46 +6062,38 @@
       <c r="B34" s="5">
         <v>29</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>109</v>
+      <c r="C34" s="23" t="s">
+        <v>107</v>
       </c>
       <c r="D34" s="13">
-        <v>4</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="16">
-        <v>1</v>
-      </c>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="16">
-        <v>1</v>
-      </c>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1">
-        <v>0.5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
       <c r="AE34" s="11"/>
       <c r="AF34" s="11"/>
       <c r="AG34" s="11"/>
@@ -6093,7 +6105,9 @@
       <c r="AM34" s="11"/>
       <c r="AN34" s="11"/>
       <c r="AO34" s="11"/>
-      <c r="AP34" s="11"/>
+      <c r="AP34" s="1">
+        <v>3</v>
+      </c>
       <c r="AQ34" s="11"/>
       <c r="AR34" s="11"/>
       <c r="AS34" s="11"/>
@@ -6136,10 +6150,10 @@
       <c r="B35" s="5">
         <v>30</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="12">
+      <c r="C35" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="13">
         <v>2</v>
       </c>
       <c r="E35" s="11"/>
@@ -6179,7 +6193,9 @@
       <c r="AM35" s="11"/>
       <c r="AN35" s="11"/>
       <c r="AO35" s="11"/>
-      <c r="AP35" s="11"/>
+      <c r="AP35" s="1">
+        <v>2</v>
+      </c>
       <c r="AQ35" s="11"/>
       <c r="AR35" s="11"/>
       <c r="AS35" s="11"/>
@@ -6222,48 +6238,50 @@
       <c r="B36" s="5">
         <v>31</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D36" s="12">
-        <v>2</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
-      <c r="W36" s="11"/>
-      <c r="X36" s="11"/>
-      <c r="Y36" s="11"/>
-      <c r="Z36" s="11"/>
-      <c r="AA36" s="11"/>
-      <c r="AB36" s="11"/>
-      <c r="AC36" s="11"/>
-      <c r="AD36" s="11"/>
-      <c r="AE36" s="11"/>
-      <c r="AF36" s="11"/>
-      <c r="AG36" s="11"/>
-      <c r="AH36" s="11"/>
-      <c r="AI36" s="11"/>
-      <c r="AJ36" s="11"/>
-      <c r="AK36" s="11"/>
-      <c r="AL36" s="11"/>
-      <c r="AM36" s="11"/>
-      <c r="AN36" s="11"/>
+      <c r="C36" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="13">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="1"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
+      <c r="AK36" s="1"/>
+      <c r="AL36" s="1"/>
+      <c r="AM36" s="1"/>
+      <c r="AN36" s="1">
+        <v>1</v>
+      </c>
       <c r="AO36" s="11"/>
       <c r="AP36" s="11"/>
       <c r="AQ36" s="11"/>
@@ -6309,49 +6327,51 @@
         <v>32</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D37" s="13">
-        <v>1</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="1">
+        <v>2</v>
+      </c>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="1"/>
-      <c r="AD37" s="1"/>
-      <c r="AE37" s="1"/>
-      <c r="AF37" s="1"/>
-      <c r="AG37" s="1"/>
-      <c r="AH37" s="1"/>
-      <c r="AI37" s="1"/>
-      <c r="AJ37" s="1"/>
-      <c r="AK37" s="1"/>
-      <c r="AL37" s="1"/>
-      <c r="AM37" s="1"/>
-      <c r="AN37" s="1">
+      <c r="Y37" s="1">
         <v>1</v>
       </c>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="11"/>
+      <c r="AI37" s="11"/>
+      <c r="AJ37" s="11"/>
+      <c r="AK37" s="11"/>
+      <c r="AL37" s="11"/>
+      <c r="AM37" s="11"/>
+      <c r="AN37" s="11"/>
       <c r="AO37" s="11"/>
       <c r="AP37" s="11"/>
       <c r="AQ37" s="11"/>
@@ -6396,11 +6416,11 @@
       <c r="B38" s="5">
         <v>33</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="13">
-        <v>3</v>
+      <c r="C38" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="15">
+        <v>1</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -6416,17 +6436,19 @@
       <c r="P38" s="11"/>
       <c r="Q38" s="11"/>
       <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11"/>
-      <c r="V38" s="1">
-        <v>2</v>
-      </c>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1">
+      <c r="S38" s="1">
         <v>1</v>
       </c>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="16">
+        <v>-1</v>
+      </c>
+      <c r="W38" s="1">
+        <v>1</v>
+      </c>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
       <c r="Z38" s="11"/>
       <c r="AA38" s="11"/>
       <c r="AB38" s="11"/>
@@ -6435,15 +6457,17 @@
       <c r="AE38" s="11"/>
       <c r="AF38" s="11"/>
       <c r="AG38" s="11"/>
-      <c r="AH38" s="11"/>
-      <c r="AI38" s="11"/>
-      <c r="AJ38" s="11"/>
-      <c r="AK38" s="11"/>
-      <c r="AL38" s="11"/>
-      <c r="AM38" s="11"/>
-      <c r="AN38" s="11"/>
-      <c r="AO38" s="11"/>
-      <c r="AP38" s="11"/>
+      <c r="AH38" s="16">
+        <v>-1</v>
+      </c>
+      <c r="AI38" s="16"/>
+      <c r="AJ38" s="16"/>
+      <c r="AK38" s="16"/>
+      <c r="AL38" s="16"/>
+      <c r="AM38" s="16"/>
+      <c r="AN38" s="16"/>
+      <c r="AO38" s="16"/>
+      <c r="AP38" s="16"/>
       <c r="AQ38" s="11"/>
       <c r="AR38" s="11"/>
       <c r="AS38" s="11"/>
@@ -6486,10 +6510,10 @@
       <c r="B39" s="5">
         <v>34</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39" s="15">
+      <c r="C39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="13">
         <v>1</v>
       </c>
       <c r="E39" s="11"/>
@@ -6506,17 +6530,11 @@
       <c r="P39" s="11"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="11"/>
-      <c r="S39" s="1">
-        <v>1</v>
-      </c>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="16">
-        <v>-1</v>
-      </c>
-      <c r="W39" s="1">
-        <v>1</v>
-      </c>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
       <c r="X39" s="11"/>
       <c r="Y39" s="11"/>
       <c r="Z39" s="11"/>
@@ -6526,16 +6544,18 @@
       <c r="AD39" s="11"/>
       <c r="AE39" s="11"/>
       <c r="AF39" s="11"/>
-      <c r="AG39" s="11"/>
-      <c r="AH39" s="16">
-        <v>-1</v>
-      </c>
-      <c r="AI39" s="16"/>
-      <c r="AJ39" s="16"/>
-      <c r="AK39" s="16"/>
-      <c r="AL39" s="16"/>
-      <c r="AM39" s="16"/>
-      <c r="AN39" s="16"/>
+      <c r="AG39" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AK39" s="11"/>
+      <c r="AL39" s="11"/>
+      <c r="AM39" s="11"/>
+      <c r="AN39" s="11"/>
       <c r="AO39" s="11"/>
       <c r="AP39" s="11"/>
       <c r="AQ39" s="11"/>
@@ -6581,7 +6601,7 @@
         <v>35</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D40" s="13">
         <v>1</v>
@@ -6611,17 +6631,15 @@
       <c r="AA40" s="11"/>
       <c r="AB40" s="11"/>
       <c r="AC40" s="11"/>
-      <c r="AD40" s="11"/>
+      <c r="AD40" s="1">
+        <v>1</v>
+      </c>
       <c r="AE40" s="11"/>
       <c r="AF40" s="11"/>
-      <c r="AG40" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="AH40" s="1"/>
-      <c r="AI40" s="1"/>
-      <c r="AJ40" s="1">
-        <v>0.5</v>
-      </c>
+      <c r="AG40" s="11"/>
+      <c r="AH40" s="11"/>
+      <c r="AI40" s="11"/>
+      <c r="AJ40" s="11"/>
       <c r="AK40" s="11"/>
       <c r="AL40" s="11"/>
       <c r="AM40" s="11"/>
@@ -6671,7 +6689,7 @@
         <v>36</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D41" s="13">
         <v>1</v>
@@ -6697,13 +6715,13 @@
       <c r="W41" s="11"/>
       <c r="X41" s="11"/>
       <c r="Y41" s="11"/>
-      <c r="Z41" s="11"/>
+      <c r="Z41" s="1">
+        <v>1</v>
+      </c>
       <c r="AA41" s="11"/>
       <c r="AB41" s="11"/>
       <c r="AC41" s="11"/>
-      <c r="AD41" s="1">
-        <v>1</v>
-      </c>
+      <c r="AD41" s="11"/>
       <c r="AE41" s="11"/>
       <c r="AF41" s="11"/>
       <c r="AG41" s="11"/>
@@ -6759,7 +6777,7 @@
         <v>37</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D42" s="13">
         <v>1</v>
@@ -6846,12 +6864,8 @@
       <c r="B43" s="5">
         <v>38</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="13">
-        <v>1</v>
-      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="12"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -6873,9 +6887,7 @@
       <c r="W43" s="11"/>
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
-      <c r="Z43" s="1">
-        <v>1</v>
-      </c>
+      <c r="Z43" s="11"/>
       <c r="AA43" s="11"/>
       <c r="AB43" s="11"/>
       <c r="AC43" s="11"/>
@@ -6934,7 +6946,9 @@
       <c r="B44" s="5">
         <v>39</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="D44" s="12"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
@@ -7016,7 +7030,9 @@
       <c r="B45" s="5">
         <v>40</v>
       </c>
-      <c r="C45" s="11"/>
+      <c r="C45" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="D45" s="12"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
@@ -7098,7 +7114,9 @@
       <c r="B46" s="5">
         <v>41</v>
       </c>
-      <c r="C46" s="11"/>
+      <c r="C46" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="D46" s="12"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
@@ -8981,10 +8999,10 @@
       <c r="CA68" s="11"/>
     </row>
     <row r="69" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B69" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="C69" s="21"/>
+      <c r="B69" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="20"/>
       <c r="D69" s="6">
         <f>SUM(D6:D68)</f>
         <v>63</v>
@@ -9019,115 +9037,115 @@
       </c>
       <c r="L69" s="7">
         <f t="shared" si="0"/>
-        <v>50.5</v>
+        <v>49.5</v>
       </c>
       <c r="M69" s="7">
         <f t="shared" si="0"/>
-        <v>50.5</v>
+        <v>49.5</v>
       </c>
       <c r="N69" s="7">
         <f t="shared" si="0"/>
-        <v>50.5</v>
+        <v>49.5</v>
       </c>
       <c r="O69" s="7">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="P69" s="7">
         <f t="shared" si="0"/>
-        <v>33.5</v>
+        <v>35.5</v>
       </c>
       <c r="Q69" s="7">
         <f t="shared" ref="Q69:AV69" si="1">P69-SUM(Q6:Q68)</f>
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="R69" s="7">
         <f t="shared" si="1"/>
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="S69" s="7">
         <f t="shared" si="1"/>
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="T69" s="7">
         <f t="shared" si="1"/>
-        <v>23.5</v>
+        <v>25.5</v>
       </c>
       <c r="U69" s="7">
         <f t="shared" si="1"/>
-        <v>20.5</v>
+        <v>22.5</v>
       </c>
       <c r="V69" s="7">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>19.5</v>
       </c>
       <c r="W69" s="7">
         <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>16</v>
       </c>
       <c r="X69" s="7">
         <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>16</v>
       </c>
       <c r="Y69" s="7">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>15</v>
       </c>
       <c r="Z69" s="7">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>13</v>
       </c>
       <c r="AA69" s="7">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>13</v>
       </c>
       <c r="AB69" s="7">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>13</v>
       </c>
       <c r="AC69" s="7">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>13</v>
       </c>
       <c r="AD69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AE69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AF69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AG69" s="7">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="AH69" s="7">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="AI69" s="7">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="AJ69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AK69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AL69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AM69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
@@ -9139,162 +9157,162 @@
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AS69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AT69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AU69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AV69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AW69" s="7">
         <f t="shared" ref="AW69:CA69" si="2">AV69-SUM(AW6:AW68)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AX69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AY69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AZ69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BA69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BB69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BC69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BD69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BE69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BF69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BG69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BH69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BI69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BJ69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BN69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BO69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BP69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BQ69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BR69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BS69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BT69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BU69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BV69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BW69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BX69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BY69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="BZ69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="CA69" s="7">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="2:79" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B70" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C70" s="20"/>
+      <c r="B70" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" s="19"/>
       <c r="D70" s="3">
         <f>SUM(D6:D68)</f>
         <v>63</v>

</xml_diff>

<commit_message>
Major revision ChatGPT. Delete user working.
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7400420D-979F-4643-9340-4A3C0B6709CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233C4E09-D46D-4337-8581-A2D841569DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -1111,16 +1111,16 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>3</c:v>
@@ -2913,8 +2913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="AP18" sqref="AP18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AR18" sqref="AR18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4589,7 +4589,7 @@
         <v>1</v>
       </c>
       <c r="AO17" s="16">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AP17" s="16"/>
       <c r="AQ17" s="16"/>
@@ -4634,10 +4634,10 @@
       <c r="B18" s="5">
         <v>13</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="13">
         <v>2</v>
       </c>
       <c r="E18" s="11"/>
@@ -4676,12 +4676,18 @@
       <c r="AJ18" s="16"/>
       <c r="AK18" s="16"/>
       <c r="AL18" s="16"/>
-      <c r="AM18" s="16"/>
-      <c r="AN18" s="16"/>
-      <c r="AO18" s="16"/>
+      <c r="AM18" s="11"/>
+      <c r="AN18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="16">
+        <v>-2</v>
+      </c>
       <c r="AP18" s="16"/>
       <c r="AQ18" s="16"/>
-      <c r="AR18" s="11"/>
+      <c r="AR18" s="1">
+        <v>2</v>
+      </c>
       <c r="AS18" s="11"/>
       <c r="AT18" s="11"/>
       <c r="AU18" s="11"/>
@@ -9151,19 +9157,19 @@
       </c>
       <c r="AN69" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AO69" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AP69" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AQ69" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AR69" s="7">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
css cleanup. removal obsolete files.
</commit_message>
<xml_diff>
--- a/documentation/MC_Burndown.xlsx
+++ b/documentation/MC_Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MunicipalC\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261960FA-057A-4800-BCBE-033719A3C701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC00D0CB-AB5C-4EFF-8525-434DDF51E441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB255D5F-88DF-47E2-A1AF-778D108B7A6B}"/>
   </bookViews>
@@ -1177,10 +1177,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>1</c:v>
@@ -2910,8 +2910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61082E50-EE00-42D2-8B67-A2DA9B04A06D}">
   <dimension ref="B2:CA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7:BJ7"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3713,11 +3713,11 @@
       <c r="BH7" s="1"/>
       <c r="BI7" s="1"/>
       <c r="BJ7" s="1"/>
-      <c r="BK7" s="1">
+      <c r="BK7" s="1"/>
+      <c r="BL7" s="1"/>
+      <c r="BM7" s="1">
         <v>1</v>
       </c>
-      <c r="BL7" s="11"/>
-      <c r="BM7" s="11"/>
       <c r="BN7" s="11"/>
       <c r="BO7" s="11"/>
       <c r="BP7" s="11"/>
@@ -6493,12 +6493,12 @@
       <c r="BH38" s="16"/>
       <c r="BI38" s="16"/>
       <c r="BJ38" s="16"/>
-      <c r="BK38" s="11"/>
-      <c r="BL38" s="11"/>
-      <c r="BM38" s="11"/>
-      <c r="BN38" s="11"/>
-      <c r="BO38" s="11"/>
-      <c r="BP38" s="11"/>
+      <c r="BK38" s="16"/>
+      <c r="BL38" s="16"/>
+      <c r="BM38" s="16"/>
+      <c r="BN38" s="16"/>
+      <c r="BO38" s="16"/>
+      <c r="BP38" s="16"/>
       <c r="BQ38" s="11"/>
       <c r="BR38" s="11"/>
       <c r="BS38" s="11"/>
@@ -9246,11 +9246,11 @@
       </c>
       <c r="BK69" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BL69" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BM69" s="7">
         <f t="shared" si="2"/>

</xml_diff>